<commit_message>
1. battleship_v5 a. Implemented queue with number of ships each player has. b. queue<string> ships, setShips(), prntQue() c. Added constructor() to prepare to implement Classes d. Changed pushName() to setSet() and reduced some redundant code e. setStack() initializes a stack with a list f. Finished docs>checklist
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/projects/project_1/documents/df_project_1_checklist.xlsx
+++ b/projects/project_1/documents/df_project_1_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_git2\projects\project_1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441346C2-078B-4AB8-89F5-D9D6F4892BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EEDEE4-6476-49E6-ACF8-DAC0372288A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EDBB2718-7706-4DA4-A008-A358616565CA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="120">
   <si>
     <t>Note:  no vectors.</t>
   </si>
@@ -252,15 +252,9 @@
     <t>https://users.cs.northwestern.edu/~riesbeck/programming/c++/stl-iterators.html</t>
   </si>
   <si>
-    <t>forward iter plus can move to previous element. --iter, iter--</t>
-  </si>
-  <si>
     <t>if itr1 and itr2 are randAccItr, then they can perform all bidirectional iterator operations, standard pointer arthimetic ops (not itr1+itr2), and comparisons</t>
   </si>
   <si>
-    <t>combines input iter and output iter. Can read and write data. They support saving and reusing. Ex: itr and next=itr; itr++. Note: A saved iterator is only valid if the underlying container is not modified. If you insert elements or otherwise change the container, using a saved iterator will have undefined behavior.</t>
-  </si>
-  <si>
     <t>two rules for making container-based code general and efficient: Never pass containers into a function. Pass iterators instead. Never return containers. Return -- or pass -- iterators instead.</t>
   </si>
   <si>
@@ -306,14 +300,52 @@
     <t>Sequence Container</t>
   </si>
   <si>
+    <t>uses encapsulated object of deque or list. Has specific set of member functions to access its elements.</t>
+  </si>
+  <si>
+    <t>LIFO                 (Last In First Out)</t>
+  </si>
+  <si>
+    <t>FIFO.                 first in first out. Insert back, pop front.</t>
+  </si>
+  <si>
+    <t>Think of stack of books.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Think waiting in line. A holder object that stores a collection of other objects. Vectors and deques can return RandomAccessIterator's. </t>
+  </si>
+  <si>
+    <t>https://en.cppreference.com/w/cpp/algorithm/min</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Arrangement Description/Notes</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   484  min({*itr, last}</t>
+  </si>
+  <si>
+    <t>Github Repo:</t>
+  </si>
+  <si>
+    <t>https://github.com/koa2019/cis17c_fall2023_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vectors and deques can return RandomAccessIterator's. </t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">return a </t>
     </r>
     <r>
@@ -344,55 +376,79 @@
     </r>
   </si>
   <si>
-    <t>.begin()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  map&lt;string, float&gt; topPlyrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  map &lt;string, float&gt;::iterator itmap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  insert_iterator&lt;std::list&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  topPlyrs.find(sName)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  copy(s.begin()</t>
-  </si>
-  <si>
-    <t>uses encapsulated object of deque or list. Has specific set of member functions to access its elements.</t>
-  </si>
-  <si>
-    <t>LIFO                 (Last In First Out)</t>
-  </si>
-  <si>
-    <t>FIFO.                 first in first out. Insert back, pop front.</t>
-  </si>
-  <si>
-    <t>Think of stack of books.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Think waiting in line. A holder object that stores a collection of other objects. Vectors and deques can return RandomAccessIterator's. </t>
-  </si>
-  <si>
-    <t>min({*itr, last}</t>
-  </si>
-  <si>
-    <t>https://en.cppreference.com/w/cpp/algorithm/min</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>Concept</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Arrangement Description/Notes</t>
+    <t>https://en.cppreference.com/w/cpp/container, https://users.cs.northwestern.edu/~riesbeck/programming/c++/stl-summary.html</t>
+  </si>
+  <si>
+    <t>Algorithms</t>
+  </si>
+  <si>
+    <t>Non-mutating algorithms</t>
+  </si>
+  <si>
+    <t>Mutating algorithms</t>
+  </si>
+  <si>
+    <t>Non-Mutating algorithms</t>
+  </si>
+  <si>
+    <t>Organization  algorithms</t>
+  </si>
+  <si>
+    <t>list return a BidirectionalIterator, but not a RandomAccessIterator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward iter plus can move to previous element. --iter, iter--, set(), begin() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">combines input iter and output iter ops. Can read and write data. They support saving and reusing. Ex: itr and next=itr; itr++. Note: A saved iterator is only valid if the underlying container is not modified. If you insert elements or otherwise change the container, using a saved iterator will have undefined behavior. ok to use with multipass algorithms. Forward only. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.lix.polytechnique.fr/~liberti/public/computing/prog/libstdc%2B%2B/ForwardIterator.html, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.boost.org/sgi/stl/trivial.html, </t>
+  </si>
+  <si>
+    <t>insert_iterator, ostream_iterator, front insert_iterator, back insert_iterator</t>
+  </si>
+  <si>
+    <t>istream_iterator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.lix.polytechnique.fr/~liberti/public/computing/prog/libstdc%2B%2B/Iterators.html </t>
+  </si>
+  <si>
+    <t>T*, list&lt;T&gt;::iterator</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T*, vector&lt;T&gt;::iterator, vector&lt;T&gt;::const_iterator,  deque&lt;T&gt;::iterator, deque&lt;T&gt;::const_iterator </t>
+  </si>
+  <si>
+    <t>T*, hash_set&lt;T&gt;::iterator</t>
+  </si>
+  <si>
+    <t>list. Refinement of Fwrd Itr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only operation that a is guaranteed to be supported is assigning a nonsingular iterator to a singular iterator. A type that is a model of Trivial Iterator may be mutable, meaning that the values referred to by objects of that type may be modified, or constant, meaning that they may not. A pointer to an object that is not part of an array.  </t>
+  </si>
+  <si>
+    <t>int*, const int*, vector</t>
+  </si>
+  <si>
+    <t>list. Refinement of Trivial Itr</t>
+  </si>
+  <si>
+    <t>set,  Refinement of Trivial Itr</t>
+  </si>
+  <si>
+    <t>list, set, map,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vectors, deques. Refinement of Bidirectional Itr</t>
   </si>
 </sst>
 </file>
@@ -522,7 +578,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,8 +591,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -895,12 +975,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,12 +1071,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -978,9 +1078,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -990,17 +1087,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1044,148 +1213,287 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1505,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C713338-5DA8-4E49-8440-D5E06C12ABCA}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1514,118 +1822,121 @@
     <col min="1" max="1" width="26.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="46.25" style="24" customWidth="1"/>
+    <col min="4" max="4" width="65.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.625" style="22" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:12" ht="21.75" thickBot="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="F4" s="38" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="F4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="61"/>
     </row>
     <row r="5" spans="1:12" ht="23.25">
       <c r="A5" s="53"/>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
       <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
       <c r="A6" s="53"/>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-    </row>
-    <row r="7" spans="1:12" ht="37.5" customHeight="1">
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+    </row>
+    <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
       <c r="A7" s="53"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="F7" s="9" t="s">
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="F7" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
     </row>
     <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="F8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="A8" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="10"/>
@@ -1636,19 +1947,19 @@
       <c r="D9" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="25"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="24" thickBot="1">
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="62"/>
+      <c r="D10" s="44"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1657,117 +1968,123 @@
       <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="45"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="66"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="23.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="37">
+        <v>548</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="23.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="26"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:12" ht="23.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="64"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:12" ht="23.25" customHeight="1">
       <c r="A16" s="13"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="58"/>
     </row>
     <row r="17" spans="1:6" ht="23.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="23" t="s">
+      <c r="B17" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="37">
+        <v>581</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="23.25">
       <c r="A18" s="14"/>
-      <c r="B18" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="23" t="s">
+      <c r="B18" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>83</v>
+      <c r="D18" s="37">
+        <v>512</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="33"/>
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1">
       <c r="A20" s="13"/>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
     </row>
     <row r="21" spans="1:6" ht="23.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="33"/>
+      <c r="D21" s="37">
+        <v>438</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="23.25">
       <c r="A22" s="14"/>
-      <c r="B22" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="33"/>
+      <c r="D22" s="37"/>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:6" ht="24" thickBot="1">
@@ -1784,241 +2101,283 @@
       <c r="A24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="F24"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="164" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="156"/>
     </row>
     <row r="25" spans="1:6" ht="23.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" ht="23.25">
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="156"/>
+    </row>
+    <row r="26" spans="1:6" ht="93.75">
       <c r="A26" s="14"/>
       <c r="B26" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="33"/>
+      <c r="D26" s="154" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="158" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="155"/>
     </row>
     <row r="27" spans="1:6" ht="23.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="23" t="s">
+      <c r="B27" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="23.25">
+      <c r="D27" s="152" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="159" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="155">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="37.5">
       <c r="A28" s="14"/>
-      <c r="B28" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="23" t="s">
+      <c r="B28" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>85</v>
+      <c r="D28" s="152" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="160" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="155">
+        <v>551</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="23.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="33"/>
+      <c r="D29" s="152" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="161" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" s="155"/>
     </row>
     <row r="30" spans="1:6" ht="23.25">
       <c r="A30" s="14"/>
-      <c r="B30" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="23" t="s">
+      <c r="B30" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="32"/>
-    </row>
-    <row r="31" spans="1:6" ht="24" thickBot="1">
+      <c r="D30" s="153" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" s="161" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="162">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="38.25" thickBot="1">
       <c r="A31" s="17"/>
-      <c r="B31" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="21" t="s">
+      <c r="B31" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="34"/>
+      <c r="D31" s="152" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="163" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="155"/>
     </row>
     <row r="32" spans="1:6" ht="24" thickBot="1">
       <c r="A32" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="52"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="70"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="19"/>
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="48"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" spans="1:4" ht="23.25">
       <c r="A34" s="14"/>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="64"/>
+      <c r="D34" s="33"/>
     </row>
     <row r="35" spans="1:4" ht="23.25">
       <c r="A35" s="14"/>
-      <c r="B35" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="23" t="s">
+      <c r="B35" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="32" t="s">
-        <v>86</v>
+      <c r="D35" s="37">
+        <v>528</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="23.25">
       <c r="A36" s="14"/>
-      <c r="B36" s="68" t="s">
+      <c r="B36" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="63" t="s">
+      <c r="C36" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="64"/>
+      <c r="D36" s="33"/>
     </row>
     <row r="37" spans="1:4" ht="23.25">
       <c r="A37" s="14"/>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="64"/>
+      <c r="D37" s="33"/>
     </row>
     <row r="38" spans="1:4" ht="23.25">
       <c r="A38" s="14"/>
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="63" t="s">
+      <c r="C38" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="64"/>
+      <c r="D38" s="33"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="14"/>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="58"/>
     </row>
     <row r="40" spans="1:4" ht="23.25">
       <c r="A40" s="14"/>
-      <c r="B40" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="23" t="s">
+      <c r="B40" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="32" t="s">
-        <v>87</v>
+      <c r="D40" s="37">
+        <v>556</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="23.25">
       <c r="A41" s="14"/>
-      <c r="B41" s="68" t="s">
+      <c r="B41" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="33"/>
     </row>
     <row r="42" spans="1:4" ht="23.25">
       <c r="A42" s="14"/>
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="64"/>
+      <c r="D42" s="33"/>
     </row>
     <row r="43" spans="1:4" ht="23.25">
       <c r="A43" s="14"/>
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="33"/>
     </row>
     <row r="44" spans="1:4" ht="23.25">
       <c r="A44" s="14"/>
-      <c r="B44" s="68" t="s">
+      <c r="B44" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="63" t="s">
+      <c r="C44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="64"/>
+      <c r="D44" s="33"/>
     </row>
     <row r="45" spans="1:4" ht="23.25">
       <c r="A45" s="14"/>
-      <c r="B45" s="68" t="s">
+      <c r="B45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="33"/>
     </row>
     <row r="46" spans="1:4" ht="23.25">
       <c r="A46" s="14"/>
-      <c r="B46" s="68" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="63" t="s">
+      <c r="B46" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="64"/>
+      <c r="D46" s="33"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="14"/>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="37"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="58"/>
     </row>
     <row r="48" spans="1:4" ht="23.25">
       <c r="A48" s="14"/>
@@ -2062,25 +2421,18 @@
     </row>
     <row r="52" spans="1:4" ht="24" thickBot="1">
       <c r="A52" s="15"/>
-      <c r="B52" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="66" t="s">
+      <c r="B52" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="67" t="s">
-        <v>93</v>
+      <c r="D52" s="41" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D7"/>
+  <mergeCells count="23">
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="F4:L4"/>
@@ -2095,524 +2447,671 @@
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{60361EF0-453D-471A-93E8-D23BF97AECCB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D102759-3B54-49C6-A2D4-1BB335BF647F}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="96" customWidth="1"/>
-    <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="56.125" style="28" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="30" customWidth="1"/>
-    <col min="6" max="6" width="53.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.75" style="30" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="70.25" style="25" customWidth="1"/>
+    <col min="5" max="5" width="17.75" style="27" customWidth="1"/>
+    <col min="6" max="6" width="60.25" style="5" customWidth="1"/>
     <col min="7" max="7" width="44.75" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="30"/>
+    <col min="8" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="72" customFormat="1" ht="58.5" customHeight="1" thickBot="1">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="58.5" customHeight="1">
+      <c r="A1" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="100" customFormat="1" ht="48" thickBot="1">
+      <c r="A2" s="125" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="128" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="125" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="120" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="121"/>
+      <c r="F2" s="122" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="121"/>
+    </row>
+    <row r="3" spans="1:7" s="84" customFormat="1" ht="34.5" customHeight="1" thickTop="1">
+      <c r="A3" s="117" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="124" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="118" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+    </row>
+    <row r="4" spans="1:7" s="84" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A4" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="130" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="123" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="83"/>
+      <c r="F4" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="83"/>
+    </row>
+    <row r="5" spans="1:7" s="90" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A5" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="123" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+    </row>
+    <row r="6" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A6" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="91" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="123" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+    </row>
+    <row r="7" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A7" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="123" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="88"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+    </row>
+    <row r="8" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A8" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="123" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="88"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="1:7" s="90" customFormat="1" ht="56.25">
+      <c r="A9" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="82"/>
+    </row>
+    <row r="10" spans="1:7" s="90" customFormat="1" ht="75">
+      <c r="A10" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="88" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="82"/>
+    </row>
+    <row r="11" spans="1:7" s="90" customFormat="1" ht="63">
+      <c r="A11" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="131" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="104" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="106"/>
+      <c r="F11" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="107" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="116" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A12" s="126" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="132" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="126" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="113" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="114"/>
+      <c r="F12" s="151" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="115"/>
+    </row>
+    <row r="13" spans="1:7" s="73" customFormat="1" ht="57" thickTop="1">
+      <c r="A13" s="108" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="109"/>
+      <c r="D13" s="110" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="111"/>
+      <c r="F13" s="150" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="112"/>
+    </row>
+    <row r="14" spans="1:7" s="73" customFormat="1" ht="36" customHeight="1">
+      <c r="A14" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="78"/>
+      <c r="D14" s="92" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="80"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+    </row>
+    <row r="15" spans="1:7" s="73" customFormat="1" ht="56.25">
+      <c r="A15" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="78"/>
+      <c r="D15" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="80"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+    </row>
+    <row r="16" spans="1:7" s="73" customFormat="1" ht="112.5">
+      <c r="A16" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="78"/>
+      <c r="D16" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="80"/>
+      <c r="F16" s="149" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="76"/>
+    </row>
+    <row r="17" spans="1:7" s="73" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A17" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="78"/>
+      <c r="D17" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="80"/>
+      <c r="F17" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="76"/>
+    </row>
+    <row r="18" spans="1:7" s="73" customFormat="1" ht="56.25">
+      <c r="A18" s="95" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="134" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="96"/>
+      <c r="D18" s="97" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="98"/>
+      <c r="F18" s="99" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="99"/>
+    </row>
+    <row r="19" spans="1:7" s="127" customFormat="1" ht="63.75" thickBot="1">
+      <c r="A19" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="93" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="93" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="94" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="94" t="s">
+      <c r="B19" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="128" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="146"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="147"/>
+      <c r="G19" s="147"/>
+    </row>
+    <row r="20" spans="1:7" s="90" customFormat="1" ht="30.75" thickTop="1">
+      <c r="A20" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="129" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="124" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="144"/>
+      <c r="E20" s="145"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+    </row>
+    <row r="21" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A21" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="93"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+    </row>
+    <row r="22" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A22" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="93"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+    </row>
+    <row r="23" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A23" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="93"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+    </row>
+    <row r="24" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A24" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="123" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="93"/>
+      <c r="E24" s="89"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+    </row>
+    <row r="25" spans="1:7" s="102" customFormat="1" ht="38.25" thickBot="1">
+      <c r="A25" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="136" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="94" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="74" customFormat="1" ht="59.25" customHeight="1">
-      <c r="A2" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A3" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="76" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="27"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="131.25">
-      <c r="A4" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="27"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="83"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="76"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="76"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="83"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="76"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="76"/>
-    </row>
-    <row r="9" spans="1:7" ht="56.25">
-      <c r="A9" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="83" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75">
-      <c r="A10" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="78" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="84" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="83" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63">
-      <c r="A11" s="95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="79" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="83" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="76"/>
-    </row>
-    <row r="13" spans="1:7" ht="75">
-      <c r="A13" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="78" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="76"/>
-    </row>
-    <row r="14" spans="1:7" ht="54">
-      <c r="A14" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="77"/>
-      <c r="F14" s="76"/>
-    </row>
-    <row r="15" spans="1:7" ht="75">
-      <c r="A15" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="83" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="76"/>
-    </row>
-    <row r="16" spans="1:7" ht="112.5">
-      <c r="A16" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" s="78" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="77"/>
-      <c r="F16" s="76"/>
-    </row>
-    <row r="17" spans="1:6" ht="37.5">
-      <c r="A17" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="77"/>
-      <c r="F17" s="76" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="56.25">
-      <c r="A18" s="78" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="78" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="77"/>
-      <c r="F18" s="76"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="95"/>
-      <c r="B19" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="88"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="76"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="95"/>
-      <c r="B20" s="87" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="76"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="95"/>
-      <c r="B21" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="76"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="95"/>
-      <c r="B22" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="88"/>
-      <c r="D22" s="89"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="76"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="95"/>
-      <c r="B23" s="87" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="88"/>
-      <c r="D23" s="89"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="76"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="95"/>
-      <c r="B24" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="76"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="95"/>
-      <c r="B25" s="87" t="s">
+      <c r="C25" s="136" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="137"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="139"/>
+      <c r="G25" s="139"/>
+    </row>
+    <row r="26" spans="1:7" s="94" customFormat="1" ht="37.5" customHeight="1" thickTop="1">
+      <c r="A26" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="140" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="88"/>
-      <c r="D25" s="89"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="76"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="95"/>
-      <c r="B26" s="87" t="s">
+      <c r="C26" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="142"/>
+      <c r="E26" s="138"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+    </row>
+    <row r="27" spans="1:7" s="94" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A27" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="140" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="88"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="76"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="95"/>
-      <c r="B27" s="87" t="s">
+      <c r="C27" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="142"/>
+      <c r="E27" s="138"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="139"/>
+    </row>
+    <row r="28" spans="1:7" s="94" customFormat="1" ht="36" customHeight="1">
+      <c r="A28" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="140" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="88"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="76"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="95"/>
-      <c r="B28" s="87" t="s">
+      <c r="C28" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="142"/>
+      <c r="E28" s="138"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+    </row>
+    <row r="29" spans="1:7" s="94" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A29" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="88"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="76"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="95"/>
-      <c r="B29" s="87" t="s">
+      <c r="C29" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="142"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+    </row>
+    <row r="30" spans="1:7" s="94" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A30" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="88"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="77"/>
-      <c r="F29" s="76"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="95"/>
-      <c r="B30" s="87" t="s">
+      <c r="C30" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="142"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
+    </row>
+    <row r="31" spans="1:7" s="94" customFormat="1" ht="45" customHeight="1">
+      <c r="A31" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="76"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="95"/>
-      <c r="B31" s="87" t="s">
+      <c r="C31" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="142"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="139"/>
+    </row>
+    <row r="32" spans="1:7" s="94" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A32" s="135" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="140" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="88"/>
-      <c r="D31" s="89"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="76"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="95"/>
-      <c r="B32" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="76"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="95"/>
-      <c r="B33" s="78" t="s">
+      <c r="C32" s="141" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="142"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="139"/>
+    </row>
+    <row r="33" spans="1:7" s="101" customFormat="1" ht="38.25" thickBot="1">
+      <c r="A33" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="83" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="143"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+    </row>
+    <row r="34" spans="1:7" s="90" customFormat="1" ht="30.75" thickTop="1">
+      <c r="A34" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="79"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="76"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="95"/>
-      <c r="B34" s="78" t="s">
+      <c r="C34" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="93"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+    </row>
+    <row r="35" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A35" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="79"/>
-      <c r="D34" s="92"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="76"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="95"/>
-      <c r="B35" s="78" t="s">
+      <c r="C35" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="93"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+    </row>
+    <row r="36" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A36" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="76"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="95"/>
-      <c r="B36" s="78" t="s">
+      <c r="C36" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="93"/>
+      <c r="E36" s="89"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+    </row>
+    <row r="37" spans="1:7" s="90" customFormat="1" ht="30">
+      <c r="A37" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="79"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="76"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="95"/>
-      <c r="B37" s="78" t="s">
+      <c r="C37" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="93"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+    </row>
+    <row r="38" spans="1:7" s="90" customFormat="1" ht="37.5">
+      <c r="A38" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="76" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="77"/>
-      <c r="F37" s="76"/>
+      <c r="C38" s="123" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="89"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B32:D32"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1" xr:uid="{CFE57316-597F-4B40-B57C-93704E5AFC13}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{BA282F4A-82B6-4F48-839A-A57D14225139}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{61D0B6B3-05D7-410B-B71D-120E25756D13}"/>
+    <hyperlink ref="F12" r:id="rId4" xr:uid="{DD851BB7-C3CD-40DC-B794-734D49EAF55C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1.	project1_convertArrays_to_STL_v6 a.	Looking highest score in map<>topPlyr b.	Passed map reference to topPlyrs() c.	Problem: Couldn’t get ostream to work in getName() with a list or a vector or with stream. 2.	project1_convertArrays_to_STL_v7 a.	Added Game class i.	Constructor: 1.	Initialized all the STL concepts in the constructor and start() 3.	battleship_v6 i.	Copied my cis17b_yahtzee_v29 because I need the game to be in classes.
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/projects/project_1/documents/df_project_1_checklist.xlsx
+++ b/projects/project_1/documents/df_project_1_checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_git2\projects\project_1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EEDEE4-6476-49E6-ACF8-DAC0372288A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E0EE5-737D-47F8-8BFF-2CA83AE031E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EDBB2718-7706-4DA4-A008-A358616565CA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="119">
   <si>
     <t>Note:  no vectors.</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Location in code/comments</t>
-  </si>
-  <si>
-    <t>□X</t>
   </si>
   <si>
     <t>shuffle</t>
@@ -331,9 +328,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   484  min({*itr, last}</t>
   </si>
   <si>
     <t>Github Repo:</t>
@@ -449,6 +443,9 @@
   </si>
   <si>
     <t xml:space="preserve"> vectors, deques. Refinement of Bidirectional Itr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   484  min({*itr, last}, max(), max_element()</t>
   </si>
 </sst>
 </file>
@@ -578,7 +575,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,6 +612,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1006,7 +1009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1123,12 +1126,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1141,6 +1138,306 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1171,329 +1468,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1813,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C713338-5DA8-4E49-8440-D5E06C12ABCA}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1828,115 +1809,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
     </row>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="147" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="A3" s="148"/>
+      <c r="B3" s="148"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="148"/>
     </row>
     <row r="4" spans="1:12" ht="21.75" thickBot="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="F4" s="59" t="s">
+      <c r="B4" s="150"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="F4" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="61"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="132"/>
     </row>
     <row r="5" spans="1:12" ht="23.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54" t="s">
+      <c r="A5" s="151"/>
+      <c r="B5" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
       <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="55" t="s">
+      <c r="A6" s="151"/>
+      <c r="B6" s="153" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="153"/>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
     </row>
     <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A7" s="53"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="F7" s="71" t="s">
+      <c r="A7" s="151"/>
+      <c r="B7" s="153"/>
+      <c r="C7" s="153"/>
+      <c r="D7" s="153"/>
+      <c r="F7" s="142" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="133"/>
     </row>
     <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A8" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="48"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
+      <c r="A8" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="144" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="133"/>
+      <c r="H8" s="133"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="133"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="10"/>
@@ -1953,13 +1934,13 @@
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="24" thickBot="1">
-      <c r="B10" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="43" t="s">
+      <c r="B10" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="42"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1968,23 +1949,23 @@
       <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="137"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="140"/>
       <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="23.25">
       <c r="A13" s="14"/>
       <c r="B13" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" s="36" t="s">
         <v>12</v>
@@ -1999,7 +1980,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="24"/>
@@ -2016,16 +1997,16 @@
     </row>
     <row r="16" spans="1:12" ht="23.25" customHeight="1">
       <c r="A16" s="13"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="129"/>
     </row>
     <row r="17" spans="1:6" ht="23.25">
       <c r="A17" s="14"/>
       <c r="B17" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="36" t="s">
         <v>16</v>
@@ -2037,7 +2018,7 @@
     <row r="18" spans="1:6" ht="23.25">
       <c r="A18" s="14"/>
       <c r="B18" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="36" t="s">
         <v>17</v>
@@ -2058,16 +2039,16 @@
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1">
       <c r="A20" s="13"/>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="129"/>
     </row>
     <row r="21" spans="1:6" ht="23.25">
       <c r="A21" s="14"/>
       <c r="B21" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>20</v>
@@ -2079,7 +2060,7 @@
     <row r="22" spans="1:6" ht="23.25">
       <c r="A22" s="14"/>
       <c r="B22" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="36" t="s">
         <v>21</v>
@@ -2101,143 +2082,139 @@
       <c r="A24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="164" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" s="156"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="126" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24"/>
     </row>
     <row r="25" spans="1:6" ht="23.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="156"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="139"/>
+      <c r="F25"/>
     </row>
     <row r="26" spans="1:6" ht="93.75">
       <c r="A26" s="14"/>
-      <c r="B26" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="148" t="s">
+      <c r="B26" s="156" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="154" t="s">
-        <v>115</v>
-      </c>
-      <c r="E26" s="158" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="155"/>
+      <c r="D26" s="125" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="23.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="35" t="s">
-        <v>89</v>
+      <c r="B27" s="156" t="s">
+        <v>88</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="152" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="159" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="155">
+        <v>60</v>
+      </c>
+      <c r="D27" s="123" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="1">
         <v>563</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="37.5">
       <c r="A28" s="14"/>
-      <c r="B28" s="35" t="s">
-        <v>89</v>
+      <c r="B28" s="156" t="s">
+        <v>88</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="152" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="160" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" s="155">
+        <v>59</v>
+      </c>
+      <c r="D28" s="123" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="1">
         <v>551</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="23.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="35" t="s">
-        <v>89</v>
+      <c r="B29" s="156" t="s">
+        <v>88</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="152" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" s="161" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="155"/>
+      <c r="D29" s="123" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="23.25">
       <c r="A30" s="14"/>
       <c r="B30" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="153" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="161" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="162">
+      <c r="D30" s="124" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="1">
         <v>557</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="38.25" thickBot="1">
       <c r="A31" s="17"/>
-      <c r="B31" s="35" t="s">
-        <v>89</v>
+      <c r="B31" s="156" t="s">
+        <v>88</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="152" t="s">
-        <v>119</v>
-      </c>
-      <c r="E31" s="163" t="s">
-        <v>111</v>
-      </c>
-      <c r="F31" s="155"/>
+      <c r="D31" s="123" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="24" thickBot="1">
       <c r="A32" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="60"/>
-      <c r="D32" s="70"/>
+      <c r="C32" s="131"/>
+      <c r="D32" s="141"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="19"/>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
+      <c r="C33" s="139"/>
+      <c r="D33" s="140"/>
     </row>
     <row r="34" spans="1:4" ht="23.25">
       <c r="A34" s="14"/>
@@ -2252,7 +2229,7 @@
     <row r="35" spans="1:4" ht="23.25">
       <c r="A35" s="14"/>
       <c r="B35" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>32</v>
@@ -2293,16 +2270,16 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="14"/>
-      <c r="B39" s="56" t="s">
+      <c r="B39" s="127" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="129"/>
     </row>
     <row r="40" spans="1:4" ht="23.25">
       <c r="A40" s="14"/>
       <c r="B40" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C40" s="36" t="s">
         <v>37</v>
@@ -2323,13 +2300,13 @@
     </row>
     <row r="42" spans="1:4" ht="23.25">
       <c r="A42" s="14"/>
-      <c r="B42" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="7" t="s">
+      <c r="B42" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="33"/>
+      <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" ht="23.25">
       <c r="A43" s="14"/>
@@ -2363,21 +2340,21 @@
     </row>
     <row r="46" spans="1:4" ht="23.25">
       <c r="A46" s="14"/>
-      <c r="B46" s="35" t="s">
-        <v>89</v>
+      <c r="B46" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D46" s="33"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="14"/>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="127" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="57"/>
-      <c r="D47" s="58"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="129"/>
     </row>
     <row r="48" spans="1:4" ht="23.25">
       <c r="A48" s="14"/>
@@ -2422,17 +2399,24 @@
     <row r="52" spans="1:4" ht="24" thickBot="1">
       <c r="A52" s="15"/>
       <c r="B52" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="154" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="41" t="s">
-        <v>90</v>
+      <c r="D52" s="155" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D7"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="F4:L4"/>
@@ -2449,13 +2433,6 @@
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{60361EF0-453D-471A-93E8-D23BF97AECCB}"/>
@@ -2471,7 +2448,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2487,624 +2464,624 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="75" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="74" t="s">
+    </row>
+    <row r="2" spans="1:7" s="72" customFormat="1" ht="48" thickBot="1">
+      <c r="A2" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="93"/>
+      <c r="F2" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="93"/>
+    </row>
+    <row r="3" spans="1:7" s="56" customFormat="1" ht="34.5" customHeight="1" thickTop="1">
+      <c r="A3" s="89" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+    </row>
+    <row r="4" spans="1:7" s="56" customFormat="1" ht="101.25" customHeight="1">
+      <c r="A4" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="102" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:7" s="62" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A5" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+    </row>
+    <row r="6" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A6" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+    </row>
+    <row r="7" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A7" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+    </row>
+    <row r="8" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A8" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+    </row>
+    <row r="9" spans="1:7" s="62" customFormat="1" ht="56.25">
+      <c r="A9" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="54"/>
+    </row>
+    <row r="10" spans="1:7" s="62" customFormat="1" ht="75">
+      <c r="A10" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="54"/>
+    </row>
+    <row r="11" spans="1:7" s="62" customFormat="1" ht="63">
+      <c r="A11" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="103" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="E11" s="78"/>
+      <c r="F11" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="79" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="88" customFormat="1" ht="27" customHeight="1" thickBot="1">
+      <c r="A12" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="100" customFormat="1" ht="48" thickBot="1">
-      <c r="A2" s="125" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="128" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="125" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="120" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="121"/>
-      <c r="F2" s="122" t="s">
+      <c r="B12" s="104" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="86"/>
+      <c r="F12" s="122" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="87"/>
+    </row>
+    <row r="13" spans="1:7" s="45" customFormat="1" ht="57" thickTop="1">
+      <c r="A13" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="81"/>
+      <c r="D13" s="82" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="83"/>
+      <c r="F13" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="84"/>
+    </row>
+    <row r="14" spans="1:7" s="45" customFormat="1" ht="36" customHeight="1">
+      <c r="A14" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+    </row>
+    <row r="15" spans="1:7" s="45" customFormat="1" ht="56.25">
+      <c r="A15" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="52"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+    </row>
+    <row r="16" spans="1:7" s="45" customFormat="1" ht="112.5">
+      <c r="A16" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="52"/>
+      <c r="F16" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="48"/>
+    </row>
+    <row r="17" spans="1:7" s="45" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A17" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="52"/>
+      <c r="F17" s="48" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="48"/>
+    </row>
+    <row r="18" spans="1:7" s="45" customFormat="1" ht="56.25">
+      <c r="A18" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="106" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="70"/>
+      <c r="F18" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="71"/>
+    </row>
+    <row r="19" spans="1:7" s="99" customFormat="1" ht="63.75" thickBot="1">
+      <c r="A19" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="121"/>
-    </row>
-    <row r="3" spans="1:7" s="84" customFormat="1" ht="34.5" customHeight="1" thickTop="1">
-      <c r="A3" s="117" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="129" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="124" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="118" t="s">
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="119"/>
+    </row>
+    <row r="20" spans="1:7" s="62" customFormat="1" ht="30.75" thickTop="1">
+      <c r="A20" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-    </row>
-    <row r="4" spans="1:7" s="84" customFormat="1" ht="101.25" customHeight="1">
-      <c r="A4" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="130" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="123" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="88" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="83"/>
-    </row>
-    <row r="5" spans="1:7" s="90" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A5" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="91" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="123" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-    </row>
-    <row r="6" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A6" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="91" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="88"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-    </row>
-    <row r="7" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A7" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="91" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="88"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-    </row>
-    <row r="8" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A8" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="91" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="88"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-    </row>
-    <row r="9" spans="1:7" s="90" customFormat="1" ht="56.25">
-      <c r="A9" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="91" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="88" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="91" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="82"/>
-    </row>
-    <row r="10" spans="1:7" s="90" customFormat="1" ht="75">
-      <c r="A10" s="85" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="91" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="86" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="88" t="s">
+      <c r="B20" s="101" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="116"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+    </row>
+    <row r="21" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A21" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="65"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+    </row>
+    <row r="22" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A22" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="65"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+    </row>
+    <row r="23" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A23" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="65"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+    </row>
+    <row r="24" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A24" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+    </row>
+    <row r="25" spans="1:7" s="74" customFormat="1" ht="38.25" thickBot="1">
+      <c r="A25" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="109"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="111"/>
+      <c r="G25" s="111"/>
+    </row>
+    <row r="26" spans="1:7" s="66" customFormat="1" ht="37.5" customHeight="1" thickTop="1">
+      <c r="A26" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="112" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="114"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
+    </row>
+    <row r="27" spans="1:7" s="66" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A27" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="112" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="114"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="111"/>
+    </row>
+    <row r="28" spans="1:7" s="66" customFormat="1" ht="36" customHeight="1">
+      <c r="A28" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="112" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="114"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="111"/>
+    </row>
+    <row r="29" spans="1:7" s="66" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A29" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="112" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="114"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+    </row>
+    <row r="30" spans="1:7" s="66" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A30" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="112" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="114"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="111"/>
+      <c r="G30" s="111"/>
+    </row>
+    <row r="31" spans="1:7" s="66" customFormat="1" ht="45" customHeight="1">
+      <c r="A31" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="112" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="114"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="111"/>
+    </row>
+    <row r="32" spans="1:7" s="66" customFormat="1" ht="40.5" customHeight="1">
+      <c r="A32" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="114"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+    </row>
+    <row r="33" spans="1:7" s="73" customFormat="1" ht="38.25" thickBot="1">
+      <c r="A33" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="115"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+    </row>
+    <row r="34" spans="1:7" s="62" customFormat="1" ht="30.75" thickTop="1">
+      <c r="A34" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="65"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+    </row>
+    <row r="35" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A35" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="65"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+    </row>
+    <row r="36" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A36" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="65"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="54"/>
+    </row>
+    <row r="37" spans="1:7" s="62" customFormat="1" ht="30">
+      <c r="A37" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="65"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+    </row>
+    <row r="38" spans="1:7" s="62" customFormat="1" ht="37.5">
+      <c r="A38" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="91" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="88" t="s">
-        <v>79</v>
-      </c>
-      <c r="G10" s="82"/>
-    </row>
-    <row r="11" spans="1:7" s="90" customFormat="1" ht="63">
-      <c r="A11" s="103" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="131" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="104" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="105" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="106"/>
-      <c r="F11" s="107" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="107" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="116" customFormat="1" ht="27" customHeight="1" thickBot="1">
-      <c r="A12" s="126" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="132" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="126" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="113" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="151" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="115"/>
-    </row>
-    <row r="13" spans="1:7" s="73" customFormat="1" ht="57" thickTop="1">
-      <c r="A13" s="108" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="133" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="110" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="111"/>
-      <c r="F13" s="150" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" s="112"/>
-    </row>
-    <row r="14" spans="1:7" s="73" customFormat="1" ht="36" customHeight="1">
-      <c r="A14" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-    </row>
-    <row r="15" spans="1:7" s="73" customFormat="1" ht="56.25">
-      <c r="A15" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="79" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="80"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-    </row>
-    <row r="16" spans="1:7" s="73" customFormat="1" ht="112.5">
-      <c r="A16" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="149" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="76"/>
-    </row>
-    <row r="17" spans="1:7" s="73" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A17" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="78"/>
-      <c r="D17" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="80"/>
-      <c r="F17" s="76" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" s="76"/>
-    </row>
-    <row r="18" spans="1:7" s="73" customFormat="1" ht="56.25">
-      <c r="A18" s="95" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="134" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="97" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="99" t="s">
-        <v>93</v>
-      </c>
-      <c r="G18" s="99"/>
-    </row>
-    <row r="19" spans="1:7" s="127" customFormat="1" ht="63.75" thickBot="1">
-      <c r="A19" s="125" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="128" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="128" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="146"/>
-      <c r="E19" s="146"/>
-      <c r="F19" s="147"/>
-      <c r="G19" s="147"/>
-    </row>
-    <row r="20" spans="1:7" s="90" customFormat="1" ht="30.75" thickTop="1">
-      <c r="A20" s="117" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="129" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="124" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="144"/>
-      <c r="E20" s="145"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="118"/>
-    </row>
-    <row r="21" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A21" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="123" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="93"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-    </row>
-    <row r="22" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A22" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="123" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="93"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-    </row>
-    <row r="23" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A23" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="123" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" s="93"/>
-      <c r="E23" s="89"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-    </row>
-    <row r="24" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A24" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" s="91" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="123" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="93"/>
-      <c r="E24" s="89"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-    </row>
-    <row r="25" spans="1:7" s="102" customFormat="1" ht="38.25" thickBot="1">
-      <c r="A25" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="136" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="136" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="139"/>
-      <c r="G25" s="139"/>
-    </row>
-    <row r="26" spans="1:7" s="94" customFormat="1" ht="37.5" customHeight="1" thickTop="1">
-      <c r="A26" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="140" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="142"/>
-      <c r="E26" s="138"/>
-      <c r="F26" s="139"/>
-      <c r="G26" s="139"/>
-    </row>
-    <row r="27" spans="1:7" s="94" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A27" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" s="140" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="142"/>
-      <c r="E27" s="138"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="139"/>
-    </row>
-    <row r="28" spans="1:7" s="94" customFormat="1" ht="36" customHeight="1">
-      <c r="A28" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="140" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="142"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="139"/>
-    </row>
-    <row r="29" spans="1:7" s="94" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A29" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" s="140" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="142"/>
-      <c r="E29" s="138"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="139"/>
-    </row>
-    <row r="30" spans="1:7" s="94" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A30" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="140" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="142"/>
-      <c r="E30" s="138"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="139"/>
-    </row>
-    <row r="31" spans="1:7" s="94" customFormat="1" ht="45" customHeight="1">
-      <c r="A31" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" s="140" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="142"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="139"/>
-    </row>
-    <row r="32" spans="1:7" s="94" customFormat="1" ht="40.5" customHeight="1">
-      <c r="A32" s="135" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="140" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="141" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" s="142"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="139"/>
-      <c r="G32" s="139"/>
-    </row>
-    <row r="33" spans="1:7" s="101" customFormat="1" ht="38.25" thickBot="1">
-      <c r="A33" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="83" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="83" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="143"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="82"/>
-    </row>
-    <row r="34" spans="1:7" s="90" customFormat="1" ht="30.75" thickTop="1">
-      <c r="A34" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="91" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="D34" s="93"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="82"/>
-    </row>
-    <row r="35" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A35" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="D35" s="93"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
-    </row>
-    <row r="36" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A36" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="91" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="D36" s="93"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
-    </row>
-    <row r="37" spans="1:7" s="90" customFormat="1" ht="30">
-      <c r="A37" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="91" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="93"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-    </row>
-    <row r="38" spans="1:7" s="90" customFormat="1" ht="37.5">
-      <c r="A38" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="E38" s="89"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Worked on cis17c project 1 write up. I broke a couple of versions when trying to convert things to classes and STL containers. cis17a_v9 has MySTL class and i converted string and a deque.
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/projects/project_1/documents/df_project_1_checklist.xlsx
+++ b/projects/project_1/documents/df_project_1_checklist.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_git2\projects\project_1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37E0EE5-737D-47F8-8BFF-2CA83AE031E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1B7D99-963F-448A-A1D0-C2BC729A2DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EDBB2718-7706-4DA4-A008-A358616565CA}"/>
   </bookViews>
   <sheets>
     <sheet name="project1" sheetId="2" r:id="rId1"/>
     <sheet name="terminology" sheetId="3" r:id="rId2"/>
+    <sheet name="nLines" sheetId="7" r:id="rId3"/>
+    <sheet name="MySTl_UML" sheetId="4" r:id="rId4"/>
+    <sheet name="Battleship_UML" sheetId="5" r:id="rId5"/>
+    <sheet name="Board_UML" sheetId="6" r:id="rId6"/>
+    <sheet name="project1 (2)" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="242">
   <si>
     <t>Note:  no vectors.</t>
   </si>
@@ -446,6 +451,375 @@
   </si>
   <si>
     <t xml:space="preserve">   484  min({*itr, last}, max(), max_element()</t>
+  </si>
+  <si>
+    <t>MySTL</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>deque&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>unsigned short</t>
+  </si>
+  <si>
+    <t>deque&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>unordered_set&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>stack&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>map&lt;string,float&gt;</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>indx</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>namSiz</t>
+  </si>
+  <si>
+    <t>nShips</t>
+  </si>
+  <si>
+    <t>ships</t>
+  </si>
+  <si>
+    <t>fnames</t>
+  </si>
+  <si>
+    <t>fnSize</t>
+  </si>
+  <si>
+    <t>topPlyrs</t>
+  </si>
+  <si>
+    <t>MySTL()</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>virtual ~MySTL()</t>
+  </si>
+  <si>
+    <t>setName(name : string) : void</t>
+  </si>
+  <si>
+    <t>getName() : string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">void setTopPlyrs() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">getTopPlyrs() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pause() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntStckFIFO() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntStckRev() : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shuffleThis() : void </t>
+  </si>
+  <si>
+    <t>string getMin() : void</t>
+  </si>
+  <si>
+    <t>setSet() : void</t>
+  </si>
+  <si>
+    <t>setShips() : void</t>
+  </si>
+  <si>
+    <t>fillGuess() : void</t>
+  </si>
+  <si>
+    <t>setDeqWthSize() : void</t>
+  </si>
+  <si>
+    <t>setStack(strings : list&lt;string&gt;&amp;) : void</t>
+  </si>
+  <si>
+    <t>set2Upper(str : string) : string 11/18/202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntDeq(nmes : deque&lt;string&gt;&amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntDeqRev(nmes : deque&lt;string&gt; &amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntMap(tPlyrPair : map&lt;string, float&gt;&amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntListFlt(hiScores : list&lt;float&gt;&amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntListStr(fnmes : list&lt;string&gt;&amp;) : void  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntQue(strings : queue&lt;string&gt; &amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prntSetStr(nameSets : unordered_set&lt;string&gt;&amp;) : void </t>
+  </si>
+  <si>
+    <t xml:space="preserve">shuffleThis(nums : deque&lt;int&gt;&amp;) : void </t>
+  </si>
+  <si>
+    <t>Battleship</t>
+  </si>
+  <si>
+    <t>MAXHITS</t>
+  </si>
+  <si>
+    <t>MAXSHIPS</t>
+  </si>
+  <si>
+    <t>p1Winner</t>
+  </si>
+  <si>
+    <t>nPlayer</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>guesBrd</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>scorecard</t>
+  </si>
+  <si>
+    <t>finalSC</t>
+  </si>
+  <si>
+    <t>const int</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>*int</t>
+  </si>
+  <si>
+    <t>**User</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Board [MINPLAYRS]</t>
+  </si>
+  <si>
+    <t>MINPLAYRS</t>
+  </si>
+  <si>
+    <t>ScoreCard [MINPLAYRS]</t>
+  </si>
+  <si>
+    <t>Battleship()</t>
+  </si>
+  <si>
+    <t>~Battlship()</t>
+  </si>
+  <si>
+    <t>play(plyrIndx : int) : void</t>
+  </si>
+  <si>
+    <t>setNPlayer() : void</t>
+  </si>
+  <si>
+    <t>setP1Winner(scorCard : ScoreCard[], name : string []) : void</t>
+  </si>
+  <si>
+    <t>selectDice(diceNum : int) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getRules() : void</t>
+  </si>
+  <si>
+    <t>displayOptions(ans : int &amp;) : void</t>
+  </si>
+  <si>
+    <t>ROWS</t>
+  </si>
+  <si>
+    <t>COLS</t>
+  </si>
+  <si>
+    <t>isP1Turn</t>
+  </si>
+  <si>
+    <t>plyrName</t>
+  </si>
+  <si>
+    <t>string[MINPLYRS]</t>
+  </si>
+  <si>
+    <t>p1GShps</t>
+  </si>
+  <si>
+    <t>p2GShps</t>
+  </si>
+  <si>
+    <t>numShp1</t>
+  </si>
+  <si>
+    <t>numShp2</t>
+  </si>
+  <si>
+    <t>count1</t>
+  </si>
+  <si>
+    <t>count2</t>
+  </si>
+  <si>
+    <t>board1</t>
+  </si>
+  <si>
+    <t>char[ROW][COLS]</t>
+  </si>
+  <si>
+    <t>board2</t>
+  </si>
+  <si>
+    <t>round</t>
+  </si>
+  <si>
+    <t>Board()</t>
+  </si>
+  <si>
+    <t>virtual ~Board()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fillGameBrd() : void</t>
+  </si>
+  <si>
+    <t>fllGArr() : void</t>
+  </si>
+  <si>
+    <t>fileSum() : void</t>
+  </si>
+  <si>
+    <t>confrmGuesBrd() : void</t>
+  </si>
+  <si>
+    <t>showGuess( p1GueIndx: int, p2GueIndx : int) : void</t>
+  </si>
+  <si>
+    <t>prntBrd(board : char arr[][COLS]) : void</t>
+  </si>
+  <si>
+    <t>fillBoard() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> prntRound() : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pause(ch='c' : char) : void</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> selectCategory(plyrIndx : int,    name : string): void</t>
+  </si>
+  <si>
+    <t>isNewHiScore(user : User &amp;,  recSize : const long) : bool</t>
+  </si>
+  <si>
+    <t>startgame(user : User&amp;,                  recSize : const long) : bool</t>
+  </si>
+  <si>
+    <t>setFinalSC(board Board &amp;) : void</t>
+  </si>
+  <si>
+    <t>setRound(rnd : int) : void</t>
+  </si>
+  <si>
+    <t>printBoard() const : void</t>
+  </si>
+  <si>
+    <t>printFinalSC(name="Player" : string) : void</t>
+  </si>
+  <si>
+    <t>plyrOppBrds(currPlyrIndx int, oppontentIndx : int ) : void</t>
+  </si>
+  <si>
+    <t>get_isSelected() const : void</t>
+  </si>
+  <si>
+    <t>battleship.h</t>
+  </si>
+  <si>
+    <t>whitespace</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>battleship.cpp</t>
+  </si>
+  <si>
+    <t>Board.h</t>
+  </si>
+  <si>
+    <t>board.cpp</t>
+  </si>
+  <si>
+    <t>User.h</t>
+  </si>
+  <si>
+    <t>Total lines</t>
+  </si>
+  <si>
+    <t>Net total lines</t>
+  </si>
+  <si>
+    <t>Battleship, MySTL, Board, User Classes</t>
+  </si>
+  <si>
+    <t>User.cpp</t>
+  </si>
+  <si>
+    <t>MySTL.h</t>
+  </si>
+  <si>
+    <t>MySTL.cpp</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Whitespace</t>
   </si>
 </sst>
 </file>
@@ -575,7 +949,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,12 +988,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1004,12 +1384,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="206">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1381,11 +1832,129 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1447,35 +2016,62 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1794,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C713338-5DA8-4E49-8440-D5E06C12ABCA}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="119" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1809,115 +2405,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="160" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
     </row>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="147" t="s">
+      <c r="A2" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A3" s="148"/>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
+      <c r="A3" s="161"/>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
     </row>
     <row r="4" spans="1:12" ht="21.75" thickBot="1">
-      <c r="A4" s="149" t="s">
+      <c r="A4" s="162" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="150"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="150"/>
-      <c r="F4" s="130" t="s">
+      <c r="B4" s="163"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="F4" s="170" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="131"/>
-      <c r="H4" s="131"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="132"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="172"/>
     </row>
     <row r="5" spans="1:12" ht="23.25">
-      <c r="A5" s="151"/>
-      <c r="B5" s="152" t="s">
+      <c r="A5" s="164"/>
+      <c r="B5" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="152"/>
-      <c r="D5" s="152"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
       <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="134" t="s">
+      <c r="G5" s="174" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="134"/>
-      <c r="L5" s="134"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A6" s="151"/>
-      <c r="B6" s="153" t="s">
+      <c r="A6" s="164"/>
+      <c r="B6" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="153"/>
-      <c r="D6" s="153"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="166"/>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="135" t="s">
+      <c r="G6" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
+      <c r="H6" s="175"/>
+      <c r="I6" s="175"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="175"/>
+      <c r="L6" s="175"/>
     </row>
     <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A7" s="151"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="153"/>
-      <c r="D7" s="153"/>
-      <c r="F7" s="142" t="s">
+      <c r="A7" s="164"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="F7" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="133" t="s">
+      <c r="G7" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="133"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="133"/>
-      <c r="K7" s="133"/>
-      <c r="L7" s="133"/>
+      <c r="H7" s="173"/>
+      <c r="I7" s="173"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="173"/>
+      <c r="L7" s="173"/>
     </row>
     <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
       <c r="A8" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="184" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="146"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="133"/>
-      <c r="J8" s="133"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="186"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="173"/>
+      <c r="H8" s="173"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="173"/>
+      <c r="L8" s="173"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="10"/>
@@ -1949,17 +2545,17 @@
       <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="136"/>
-      <c r="C11" s="136"/>
-      <c r="D11" s="137"/>
+      <c r="B11" s="176"/>
+      <c r="C11" s="176"/>
+      <c r="D11" s="177"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="138" t="s">
+      <c r="B12" s="178" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="139"/>
-      <c r="D12" s="140"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="180"/>
       <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="23.25">
@@ -1997,11 +2593,11 @@
     </row>
     <row r="16" spans="1:12" ht="23.25" customHeight="1">
       <c r="A16" s="13"/>
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="128"/>
-      <c r="D16" s="129"/>
+      <c r="C16" s="168"/>
+      <c r="D16" s="169"/>
     </row>
     <row r="17" spans="1:6" ht="23.25">
       <c r="A17" s="14"/>
@@ -2039,11 +2635,11 @@
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1">
       <c r="A20" s="13"/>
-      <c r="B20" s="127" t="s">
+      <c r="B20" s="167" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="128"/>
-      <c r="D20" s="129"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="169"/>
     </row>
     <row r="21" spans="1:6" ht="23.25">
       <c r="A21" s="14"/>
@@ -2082,32 +2678,32 @@
       <c r="A24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="136"/>
-      <c r="C24" s="136"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="126" t="s">
+      <c r="B24" s="176"/>
+      <c r="C24" s="176"/>
+      <c r="D24" s="176"/>
+      <c r="E24" s="125" t="s">
         <v>108</v>
       </c>
       <c r="F24"/>
     </row>
     <row r="25" spans="1:6" ht="23.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="138" t="s">
+      <c r="B25" s="178" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="139"/>
-      <c r="D25" s="139"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="179"/>
       <c r="F25"/>
     </row>
     <row r="26" spans="1:6" ht="93.75">
       <c r="A26" s="14"/>
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="125" t="s">
+      <c r="D26" s="205" t="s">
         <v>113</v>
       </c>
       <c r="E26" s="25" t="s">
@@ -2116,7 +2712,7 @@
     </row>
     <row r="27" spans="1:6" ht="23.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="35" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="36" t="s">
@@ -2134,7 +2730,7 @@
     </row>
     <row r="28" spans="1:6" ht="37.5">
       <c r="A28" s="14"/>
-      <c r="B28" s="156" t="s">
+      <c r="B28" s="35" t="s">
         <v>88</v>
       </c>
       <c r="C28" s="36" t="s">
@@ -2152,7 +2748,7 @@
     </row>
     <row r="29" spans="1:6" ht="23.25">
       <c r="A29" s="14"/>
-      <c r="B29" s="156" t="s">
+      <c r="B29" s="35" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="36" t="s">
@@ -2185,7 +2781,7 @@
     </row>
     <row r="31" spans="1:6" ht="38.25" thickBot="1">
       <c r="A31" s="17"/>
-      <c r="B31" s="156" t="s">
+      <c r="B31" s="35" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="38" t="s">
@@ -2202,19 +2798,19 @@
       <c r="A32" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="171" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="131"/>
-      <c r="D32" s="141"/>
+      <c r="C32" s="171"/>
+      <c r="D32" s="181"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="19"/>
-      <c r="B33" s="138" t="s">
+      <c r="B33" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="139"/>
-      <c r="D33" s="140"/>
+      <c r="C33" s="179"/>
+      <c r="D33" s="180"/>
     </row>
     <row r="34" spans="1:4" ht="23.25">
       <c r="A34" s="14"/>
@@ -2270,11 +2866,11 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="14"/>
-      <c r="B39" s="127" t="s">
+      <c r="B39" s="167" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="128"/>
-      <c r="D39" s="129"/>
+      <c r="C39" s="168"/>
+      <c r="D39" s="169"/>
     </row>
     <row r="40" spans="1:4" ht="23.25">
       <c r="A40" s="14"/>
@@ -2350,11 +2946,11 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="14"/>
-      <c r="B47" s="127" t="s">
+      <c r="B47" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="128"/>
-      <c r="D47" s="129"/>
+      <c r="C47" s="168"/>
+      <c r="D47" s="169"/>
     </row>
     <row r="48" spans="1:4" ht="23.25">
       <c r="A48" s="14"/>
@@ -2401,22 +2997,15 @@
       <c r="B52" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="154" t="s">
+      <c r="C52" s="126" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="155" t="s">
+      <c r="D52" s="127" t="s">
         <v>118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D7"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="F4:L4"/>
@@ -2433,6 +3022,13 @@
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{60361EF0-453D-471A-93E8-D23BF97AECCB}"/>
@@ -3092,4 +3688,1902 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8959F71E-0972-4D12-A3E9-F77A77A4DF8C}">
+  <dimension ref="B2:F26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="138" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="27"/>
+    <col min="2" max="2" width="12.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="138"/>
+    <col min="4" max="4" width="9" style="27"/>
+    <col min="5" max="5" width="13.125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="27" customWidth="1"/>
+    <col min="8" max="8" width="12.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="47.25" customHeight="1">
+      <c r="E2" s="187" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" s="187"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="138">
+        <v>54</v>
+      </c>
+      <c r="E3" s="139" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="142">
+        <f>SUM(C3,C6,C12,C15,C9,C18,C21,C24)</f>
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="138">
+        <v>-8</v>
+      </c>
+      <c r="E4" s="140" t="s">
+        <v>240</v>
+      </c>
+      <c r="F4" s="141">
+        <f>SUM(C4,C7,C10,C13,C16,C19,C22,C25)*-1</f>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="138">
+        <v>-9</v>
+      </c>
+      <c r="E5" s="139" t="s">
+        <v>241</v>
+      </c>
+      <c r="F5" s="143">
+        <f>SUM(C5,C8,C11,C14,C17,C20,C23,C26)*-1</f>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="138">
+        <v>359</v>
+      </c>
+      <c r="E6" s="144" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="145">
+        <f>F3-F4-F5</f>
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C7" s="138">
+        <v>-83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" s="138">
+        <v>-67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="138">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" s="138">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="138">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="138">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13" s="138">
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14" s="138">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="138">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" s="138">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="138">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="138">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" s="138">
+        <v>-143</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="138">
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" s="138">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="138">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="138">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="138">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="138">
+        <v>-49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="138">
+        <v>-82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623B27F6-7E7F-4F84-8B3B-52A337061DED}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:I40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="27"/>
+    <col min="2" max="2" width="3.75" style="128" customWidth="1"/>
+    <col min="3" max="3" width="7.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="1.875" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.25" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="16.5" thickBot="1"/>
+    <row r="3" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B3" s="194" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="132" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="134" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="134" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="134" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="134" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="137"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="134" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="134" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="27" customHeight="1" thickBot="1">
+      <c r="B14" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="136" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18.75" customHeight="1">
+      <c r="B15" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="190" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="191"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="188" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="189"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="188" t="s">
+        <v>142</v>
+      </c>
+      <c r="D17" s="189"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B18" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="188" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="189"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B19" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="188" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="189"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B20" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="188" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="189"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B21" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="188" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="189"/>
+    </row>
+    <row r="22" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B22" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="188" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="189"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="188" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="189"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="188" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="189"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B25" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="188" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" s="189"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B26" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="188" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="189"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="188" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="189"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="188" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="189"/>
+    </row>
+    <row r="29" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B29" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="188" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="189"/>
+    </row>
+    <row r="30" spans="2:4" ht="33" customHeight="1">
+      <c r="B30" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="188" t="s">
+        <v>159</v>
+      </c>
+      <c r="D30" s="189"/>
+    </row>
+    <row r="31" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B31" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="188" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="189"/>
+    </row>
+    <row r="32" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B32" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="188" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" s="189"/>
+    </row>
+    <row r="33" spans="2:4" ht="34.5" customHeight="1">
+      <c r="B33" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="188" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="189"/>
+    </row>
+    <row r="34" spans="2:4" ht="32.25" customHeight="1">
+      <c r="B34" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="188" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="189"/>
+    </row>
+    <row r="35" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B35" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="188" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="189"/>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B36" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="188" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="189"/>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B37" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" s="188" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="189"/>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B38" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="188" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="189"/>
+    </row>
+    <row r="39" spans="2:4" ht="37.5" customHeight="1">
+      <c r="B39" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="188" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="189"/>
+    </row>
+    <row r="40" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B40" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="192" t="s">
+        <v>147</v>
+      </c>
+      <c r="D40" s="193"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup scale="94" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7190C4-D563-4B4F-92F4-8A7D77AC9417}">
+  <dimension ref="B2:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="27"/>
+    <col min="2" max="2" width="1.875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="16.5" thickBot="1"/>
+    <row r="3" spans="2:4" ht="16.5" thickBot="1">
+      <c r="B3" s="194" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="132" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="134" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="134" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="134" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="134" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="134" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="16.5" thickBot="1">
+      <c r="B14" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="129" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" s="136" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="131" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="190" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="191"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="188" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="189"/>
+    </row>
+    <row r="17" spans="2:4" ht="34.5" customHeight="1">
+      <c r="B17" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="188" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" s="189"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="188" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="189"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="188" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="189"/>
+    </row>
+    <row r="20" spans="2:4" ht="39" customHeight="1">
+      <c r="B20" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="188" t="s">
+        <v>188</v>
+      </c>
+      <c r="D20" s="189"/>
+    </row>
+    <row r="21" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B21" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="188" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="189"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="188" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="189"/>
+    </row>
+    <row r="23" spans="2:4" ht="37.5" customHeight="1">
+      <c r="B23" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="188" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="189"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="188" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="189"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="188" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="189"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="188" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="189"/>
+    </row>
+    <row r="27" spans="2:4" ht="16.5" thickBot="1">
+      <c r="B27" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="192" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="193"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839FF864-39E4-47C0-BA14-903CC1A36A5B}">
+  <dimension ref="B2:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="B3:D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9" style="27"/>
+    <col min="2" max="2" width="1.875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="16.5" thickBot="1"/>
+    <row r="3" spans="2:6" ht="16.5" thickBot="1">
+      <c r="B3" s="194" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="130" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="132" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="134" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="134" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="134" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" s="134" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="134" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="16.5" thickBot="1">
+      <c r="B16" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="129" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="136" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="131" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="190" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="191"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="188" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" s="189"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="188" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="189"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="188" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="189"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="188" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="189"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="188" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="189"/>
+    </row>
+    <row r="23" spans="2:4" ht="36" customHeight="1">
+      <c r="B23" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="188" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" s="189"/>
+    </row>
+    <row r="24" spans="2:4" ht="32.25" customHeight="1">
+      <c r="B24" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="188" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="189"/>
+    </row>
+    <row r="25" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B25" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="188" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="189"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="188" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" s="189"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="188" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="189"/>
+    </row>
+    <row r="28" spans="2:4" ht="29.25" customHeight="1">
+      <c r="B28" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="188" t="s">
+        <v>221</v>
+      </c>
+      <c r="D28" s="189"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="188" t="s">
+        <v>222</v>
+      </c>
+      <c r="D29" s="189"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="133" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="188" t="s">
+        <v>223</v>
+      </c>
+      <c r="D30" s="189"/>
+    </row>
+    <row r="31" spans="2:4" ht="33.75" customHeight="1" thickBot="1">
+      <c r="B31" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="192" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" s="193"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F16840-50DC-4E6F-A125-B5573596E681}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L51"/>
+  <sheetViews>
+    <sheetView topLeftCell="B3" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57" style="4" customWidth="1"/>
+    <col min="5" max="5" width="69.625" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="23.25">
+      <c r="A1" s="160" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+    </row>
+    <row r="2" spans="1:12" ht="23.25">
+      <c r="A2" s="160" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" thickBot="1">
+      <c r="A3" s="162" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="154"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
+    </row>
+    <row r="4" spans="1:12" ht="23.25">
+      <c r="A4" s="200"/>
+      <c r="B4" s="202" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="202"/>
+      <c r="D4" s="203"/>
+      <c r="F4" s="152"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A5" s="201"/>
+      <c r="B5" s="166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="166"/>
+      <c r="D5" s="204"/>
+      <c r="F5" s="152"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A6" s="201"/>
+      <c r="B6" s="166"/>
+      <c r="C6" s="166"/>
+      <c r="D6" s="204"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A7" s="146" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="197" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="198"/>
+      <c r="D7" s="199"/>
+      <c r="F7" s="153"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" ht="24" thickBot="1">
+      <c r="A9" s="155"/>
+      <c r="B9" s="147" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="148" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="149"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="47.25" thickBot="1">
+      <c r="A10" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="176"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="177"/>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="23.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="178" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="179"/>
+      <c r="D11" s="180"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:12" ht="23.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="33">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="23.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="150"/>
+    </row>
+    <row r="14" spans="1:12" ht="23.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="33"/>
+    </row>
+    <row r="15" spans="1:12" ht="23.25" customHeight="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="167" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="168"/>
+      <c r="D15" s="169"/>
+    </row>
+    <row r="16" spans="1:12" ht="23.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="33">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="23.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="33">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="23.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:6" ht="23.25" customHeight="1">
+      <c r="A19" s="13"/>
+      <c r="B19" s="167" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="168"/>
+      <c r="D19" s="169"/>
+    </row>
+    <row r="20" spans="1:6" ht="23.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="33">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="23.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="33"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" thickBot="1">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="34"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" thickBot="1">
+      <c r="A23" s="159" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="176"/>
+      <c r="C23" s="176"/>
+      <c r="D23" s="177"/>
+      <c r="E23" s="1"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6" ht="23.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="178" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="179"/>
+      <c r="D24" s="180"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" ht="23.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="156" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="25"/>
+    </row>
+    <row r="26" spans="1:6" ht="23.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="23.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="44"/>
+    </row>
+    <row r="28" spans="1:6" ht="23.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="23.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="157" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="24" thickBot="1">
+      <c r="A30" s="17"/>
+      <c r="B30" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:6" ht="24" thickBot="1">
+      <c r="A31" s="159" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="171" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="171"/>
+      <c r="D31" s="181"/>
+    </row>
+    <row r="32" spans="1:6" s="22" customFormat="1">
+      <c r="A32" s="19"/>
+      <c r="B32" s="178" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="179"/>
+      <c r="D32" s="180"/>
+    </row>
+    <row r="33" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="33"/>
+    </row>
+    <row r="34" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="33">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="33"/>
+    </row>
+    <row r="36" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="33"/>
+    </row>
+    <row r="37" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" s="33"/>
+    </row>
+    <row r="38" spans="1:4" s="22" customFormat="1">
+      <c r="A38" s="14"/>
+      <c r="B38" s="167" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="168"/>
+      <c r="D38" s="169"/>
+    </row>
+    <row r="39" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="33">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="33"/>
+    </row>
+    <row r="41" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="33"/>
+    </row>
+    <row r="42" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" s="33"/>
+    </row>
+    <row r="43" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="33"/>
+    </row>
+    <row r="44" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="33"/>
+    </row>
+    <row r="45" spans="1:4" s="22" customFormat="1" ht="24" thickBot="1">
+      <c r="A45" s="14"/>
+      <c r="B45" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="33"/>
+    </row>
+    <row r="46" spans="1:4" s="22" customFormat="1">
+      <c r="A46" s="14"/>
+      <c r="B46" s="167" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="168"/>
+      <c r="D46" s="169"/>
+    </row>
+    <row r="47" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="33"/>
+    </row>
+    <row r="48" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="33"/>
+    </row>
+    <row r="49" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="33"/>
+    </row>
+    <row r="50" spans="1:4" s="22" customFormat="1" ht="23.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="33"/>
+    </row>
+    <row r="51" spans="1:4" s="22" customFormat="1" ht="24" thickBot="1">
+      <c r="A51" s="15"/>
+      <c r="B51" s="151" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="126" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" s="127" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{48A79B56-9EDB-4A9B-992E-539D7A011C79}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="56" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cis17A_v9 was working. I made a copy of it called cis17c_project_1_v8 and then it wanted to crash. i dont know what happened.
Signed-off-by: koa2019 <no-reply>
</commit_message>
<xml_diff>
--- a/projects/project_1/documents/df_project_1_checklist.xlsx
+++ b/projects/project_1/documents/df_project_1_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanYell\Documents\cis17c_git2\projects\project_1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1B7D99-963F-448A-A1D0-C2BC729A2DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E0AE9E-FB04-441F-8316-3F182694B7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EDBB2718-7706-4DA4-A008-A358616565CA}"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="22185" windowHeight="17400" xr2:uid="{EDBB2718-7706-4DA4-A008-A358616565CA}"/>
   </bookViews>
   <sheets>
     <sheet name="project1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="MySTl_UML" sheetId="4" r:id="rId4"/>
     <sheet name="Battleship_UML" sheetId="5" r:id="rId5"/>
     <sheet name="Board_UML" sheetId="6" r:id="rId6"/>
-    <sheet name="project1 (2)" sheetId="8" r:id="rId7"/>
+    <sheet name="project1 (2)" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="248">
   <si>
     <t>Note:  no vectors.</t>
   </si>
@@ -429,30 +429,9 @@
     <t>T*, hash_set&lt;T&gt;::iterator</t>
   </si>
   <si>
-    <t>list. Refinement of Fwrd Itr</t>
-  </si>
-  <si>
     <t xml:space="preserve">The only operation that a is guaranteed to be supported is assigning a nonsingular iterator to a singular iterator. A type that is a model of Trivial Iterator may be mutable, meaning that the values referred to by objects of that type may be modified, or constant, meaning that they may not. A pointer to an object that is not part of an array.  </t>
   </si>
   <si>
-    <t>int*, const int*, vector</t>
-  </si>
-  <si>
-    <t>list. Refinement of Trivial Itr</t>
-  </si>
-  <si>
-    <t>set,  Refinement of Trivial Itr</t>
-  </si>
-  <si>
-    <t>list, set, map,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vectors, deques. Refinement of Bidirectional Itr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   484  min({*itr, last}, max(), max_element()</t>
-  </si>
-  <si>
     <t>MySTL</t>
   </si>
   <si>
@@ -820,13 +799,52 @@
   </si>
   <si>
     <t>Whitespace</t>
+  </si>
+  <si>
+    <t>See MySTL.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   221  min, 121 max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">163, </t>
+  </si>
+  <si>
+    <t>168, 243</t>
+  </si>
+  <si>
+    <t>173, 312</t>
+  </si>
+  <si>
+    <t>477, 452</t>
+  </si>
+  <si>
+    <t>177, 178, list. Refinement of Trivial Itr</t>
+  </si>
+  <si>
+    <t>172, 244. Default itr for list. Refinement of Fwrd Itr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 313, 263. Default itr for vectors, deques. Refinement of Bidirectional Itr</t>
+  </si>
+  <si>
+    <t>213, 286, 320, 344.  Refinement of Trivial Itr</t>
+  </si>
+  <si>
+    <t>320. int*, const int*, vector</t>
+  </si>
+  <si>
+    <t>265, 463</t>
+  </si>
+  <si>
+    <t>300, 311, 174. list, set, map,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -948,6 +966,14 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -999,7 +1025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1272,19 +1298,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1455,12 +1468,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1513,16 +1550,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1559,7 +1596,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1571,7 +1608,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1580,13 +1617,13 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1595,10 +1632,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1658,43 +1695,43 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1712,18 +1749,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1733,13 +1770,13 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1748,73 +1785,73 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1823,7 +1860,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1832,14 +1869,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1847,25 +1878,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1895,44 +1926,49 @@
     <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1956,121 +1992,244 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2390,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C713338-5DA8-4E49-8440-D5E06C12ABCA}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2405,115 +2564,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
+      <c r="B1" s="159"/>
+      <c r="C1" s="159"/>
+      <c r="D1" s="159"/>
     </row>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
     </row>
     <row r="3" spans="1:12" ht="19.5" thickBot="1">
-      <c r="A3" s="161"/>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
+      <c r="A3" s="160"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
     </row>
     <row r="4" spans="1:12" ht="21.75" thickBot="1">
-      <c r="A4" s="162" t="s">
+      <c r="A4" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="163"/>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="F4" s="170" t="s">
+      <c r="B4" s="162"/>
+      <c r="C4" s="162"/>
+      <c r="D4" s="162"/>
+      <c r="F4" s="145" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
-      <c r="K4" s="171"/>
-      <c r="L4" s="172"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="147"/>
     </row>
     <row r="5" spans="1:12" ht="23.25">
-      <c r="A5" s="164"/>
-      <c r="B5" s="165" t="s">
+      <c r="A5" s="163"/>
+      <c r="B5" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="165"/>
-      <c r="D5" s="165"/>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
       <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="174" t="s">
+      <c r="G5" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="174"/>
-      <c r="I5" s="174"/>
-      <c r="J5" s="174"/>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A6" s="164"/>
-      <c r="B6" s="166" t="s">
+      <c r="A6" s="163"/>
+      <c r="B6" s="165" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="166"/>
-      <c r="D6" s="166"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="175" t="s">
+      <c r="G6" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="175"/>
-      <c r="I6" s="175"/>
-      <c r="J6" s="175"/>
-      <c r="K6" s="175"/>
-      <c r="L6" s="175"/>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="150"/>
     </row>
     <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A7" s="164"/>
-      <c r="B7" s="166"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="F7" s="182" t="s">
+      <c r="A7" s="163"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="F7" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="173" t="s">
+      <c r="G7" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="173"/>
-      <c r="I7" s="173"/>
-      <c r="J7" s="173"/>
-      <c r="K7" s="173"/>
-      <c r="L7" s="173"/>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
+      <c r="L7" s="148"/>
     </row>
     <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
       <c r="A8" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="184" t="s">
+      <c r="B8" s="156" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="185"/>
-      <c r="D8" s="186"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="173"/>
-      <c r="H8" s="173"/>
-      <c r="I8" s="173"/>
-      <c r="J8" s="173"/>
-      <c r="K8" s="173"/>
-      <c r="L8" s="173"/>
+      <c r="C8" s="157"/>
+      <c r="D8" s="158"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="148"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="148"/>
+      <c r="K8" s="148"/>
+      <c r="L8" s="148"/>
     </row>
     <row r="9" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="10"/>
@@ -2545,17 +2704,19 @@
       <c r="A11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="176"/>
-      <c r="C11" s="176"/>
-      <c r="D11" s="177"/>
+      <c r="B11" s="151"/>
+      <c r="C11" s="151"/>
+      <c r="D11" s="152"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="178" t="s">
+      <c r="B12" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="179"/>
-      <c r="D12" s="180"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="179" t="s">
+        <v>235</v>
+      </c>
       <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:12" ht="23.25">
@@ -2566,8 +2727,8 @@
       <c r="C13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="37">
-        <v>548</v>
+      <c r="D13" s="37" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="23.25">
@@ -2593,11 +2754,13 @@
     </row>
     <row r="16" spans="1:12" ht="23.25" customHeight="1">
       <c r="A16" s="13"/>
-      <c r="B16" s="167" t="s">
+      <c r="B16" s="180" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="168"/>
-      <c r="D16" s="169"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="179" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="23.25">
       <c r="A17" s="14"/>
@@ -2607,8 +2770,8 @@
       <c r="C17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="37">
-        <v>581</v>
+      <c r="D17" s="37" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="23.25">
@@ -2620,7 +2783,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="37">
-        <v>512</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.25">
@@ -2635,11 +2798,13 @@
     </row>
     <row r="20" spans="1:6" ht="23.25" customHeight="1">
       <c r="A20" s="13"/>
-      <c r="B20" s="167" t="s">
+      <c r="B20" s="180" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="168"/>
-      <c r="D20" s="169"/>
+      <c r="C20" s="181"/>
+      <c r="D20" s="179" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="23.25">
       <c r="A21" s="14"/>
@@ -2650,7 +2815,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="37">
-        <v>438</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="23.25">
@@ -2661,7 +2826,9 @@
       <c r="C22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="37"/>
+      <c r="D22" s="37" t="s">
+        <v>246</v>
+      </c>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:6" ht="24" thickBot="1">
@@ -2678,9 +2845,9 @@
       <c r="A24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="176"/>
-      <c r="C24" s="176"/>
-      <c r="D24" s="176"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="151"/>
+      <c r="D24" s="151"/>
       <c r="E24" s="125" t="s">
         <v>108</v>
       </c>
@@ -2688,11 +2855,13 @@
     </row>
     <row r="25" spans="1:6" ht="23.25">
       <c r="A25" s="16"/>
-      <c r="B25" s="178" t="s">
+      <c r="B25" s="182" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="179"/>
-      <c r="D25" s="179"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="179" t="s">
+        <v>235</v>
+      </c>
       <c r="F25"/>
     </row>
     <row r="26" spans="1:6" ht="93.75">
@@ -2703,11 +2872,11 @@
       <c r="C26" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="205" t="s">
-        <v>113</v>
+      <c r="D26" s="144" t="s">
+        <v>245</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="23.25">
@@ -2719,7 +2888,7 @@
         <v>60</v>
       </c>
       <c r="D27" s="123" t="s">
-        <v>115</v>
+        <v>244</v>
       </c>
       <c r="E27" s="22" t="s">
         <v>105</v>
@@ -2737,7 +2906,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="123" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="E28" s="44" t="s">
         <v>104</v>
@@ -2755,7 +2924,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="123" t="s">
-        <v>114</v>
+        <v>241</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>110</v>
@@ -2770,7 +2939,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="124" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>107</v>
@@ -2788,7 +2957,7 @@
         <v>27</v>
       </c>
       <c r="D31" s="123" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
       <c r="E31" s="25" t="s">
         <v>109</v>
@@ -2798,19 +2967,21 @@
       <c r="A32" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="171" t="s">
+      <c r="B32" s="146" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="171"/>
-      <c r="D32" s="181"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="153"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="19"/>
-      <c r="B33" s="178" t="s">
+      <c r="B33" s="177" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="179"/>
-      <c r="D33" s="180"/>
+      <c r="C33" s="178"/>
+      <c r="D33" s="179" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="23.25">
       <c r="A34" s="14"/>
@@ -2831,7 +3002,7 @@
         <v>32</v>
       </c>
       <c r="D35" s="37">
-        <v>528</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="23.25">
@@ -2866,11 +3037,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="14"/>
-      <c r="B39" s="167" t="s">
+      <c r="B39" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="168"/>
-      <c r="D39" s="169"/>
+      <c r="C39" s="181"/>
+      <c r="D39" s="179" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="23.25">
       <c r="A40" s="14"/>
@@ -2880,8 +3053,8 @@
       <c r="C40" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="37">
-        <v>556</v>
+      <c r="D40" s="37" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="23.25">
@@ -2902,7 +3075,9 @@
       <c r="C42" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="37"/>
+      <c r="D42" s="37">
+        <v>427</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="23.25">
       <c r="A43" s="14"/>
@@ -2936,21 +3111,25 @@
     </row>
     <row r="46" spans="1:4" ht="23.25">
       <c r="A46" s="14"/>
-      <c r="B46" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="33"/>
+      <c r="D46" s="37" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="14"/>
-      <c r="B47" s="167" t="s">
+      <c r="B47" s="180" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="168"/>
-      <c r="D47" s="169"/>
+      <c r="C47" s="181"/>
+      <c r="D47" s="179" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="23.25">
       <c r="A48" s="14"/>
@@ -2997,31 +3176,16 @@
       <c r="B52" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="126" t="s">
+      <c r="C52" s="184" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="127" t="s">
-        <v>118</v>
+      <c r="D52" s="185" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="G7:L8"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="B8:D8"/>
+  <mergeCells count="17">
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
@@ -3029,6 +3193,15 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D7"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="G7:L8"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{60361EF0-453D-471A-93E8-D23BF97AECCB}"/>
@@ -3702,7 +3875,7 @@
   <cols>
     <col min="1" max="1" width="9" style="27"/>
     <col min="2" max="2" width="12.375" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="138"/>
+    <col min="3" max="3" width="9" style="136"/>
     <col min="4" max="4" width="9" style="27"/>
     <col min="5" max="5" width="13.125" style="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.875" style="27" bestFit="1" customWidth="1"/>
@@ -3712,228 +3885,228 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="47.25" customHeight="1">
-      <c r="E2" s="187" t="s">
-        <v>236</v>
-      </c>
-      <c r="F2" s="187"/>
+      <c r="E2" s="166" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="166"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="136">
+        <v>54</v>
+      </c>
+      <c r="E3" s="137" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="138">
-        <v>54</v>
-      </c>
-      <c r="E3" s="139" t="s">
-        <v>234</v>
-      </c>
-      <c r="F3" s="142">
+      <c r="F3" s="140">
         <f>SUM(C3,C6,C12,C15,C9,C18,C21,C24)</f>
         <v>1965</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="138">
+        <v>222</v>
+      </c>
+      <c r="C4" s="136">
         <v>-8</v>
       </c>
-      <c r="E4" s="140" t="s">
-        <v>240</v>
-      </c>
-      <c r="F4" s="141">
+      <c r="E4" s="138" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="139">
         <f>SUM(C4,C7,C10,C13,C16,C19,C22,C25)*-1</f>
         <v>444</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" s="138">
+        <v>221</v>
+      </c>
+      <c r="C5" s="136">
         <v>-9</v>
       </c>
-      <c r="E5" s="139" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="143">
+      <c r="E5" s="137" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="141">
         <f>SUM(C5,C8,C11,C14,C17,C20,C23,C26)*-1</f>
         <v>269</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" s="138">
+        <v>223</v>
+      </c>
+      <c r="C6" s="136">
         <v>359</v>
       </c>
-      <c r="E6" s="144" t="s">
-        <v>235</v>
-      </c>
-      <c r="F6" s="145">
+      <c r="E6" s="142" t="s">
+        <v>228</v>
+      </c>
+      <c r="F6" s="143">
         <f>F3-F4-F5</f>
         <v>1252</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C7" s="138">
+        <v>222</v>
+      </c>
+      <c r="C7" s="136">
         <v>-83</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C8" s="138">
+        <v>221</v>
+      </c>
+      <c r="C8" s="136">
         <v>-67</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="138">
+        <v>224</v>
+      </c>
+      <c r="C9" s="136">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C10" s="138">
+        <v>222</v>
+      </c>
+      <c r="C10" s="136">
         <v>-25</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C11" s="138">
+        <v>221</v>
+      </c>
+      <c r="C11" s="136">
         <v>-5</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="C12" s="138">
+        <v>225</v>
+      </c>
+      <c r="C12" s="136">
         <v>234</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="138">
+        <v>222</v>
+      </c>
+      <c r="C13" s="136">
         <v>-120</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C14" s="138">
+        <v>221</v>
+      </c>
+      <c r="C14" s="136">
         <v>-28</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="C15" s="138">
+        <v>226</v>
+      </c>
+      <c r="C15" s="136">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" s="138">
+        <v>222</v>
+      </c>
+      <c r="C16" s="136">
         <v>-10</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C17" s="138">
+        <v>221</v>
+      </c>
+      <c r="C17" s="136">
         <v>-17</v>
       </c>
     </row>
     <row r="18" spans="2:3">
       <c r="B18" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="C18" s="138">
+        <v>230</v>
+      </c>
+      <c r="C18" s="136">
         <v>638</v>
       </c>
     </row>
     <row r="19" spans="2:3">
       <c r="B19" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C19" s="138">
+        <v>222</v>
+      </c>
+      <c r="C19" s="136">
         <v>-143</v>
       </c>
     </row>
     <row r="20" spans="2:3">
       <c r="B20" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C20" s="138">
+        <v>221</v>
+      </c>
+      <c r="C20" s="136">
         <v>-56</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="C21" s="138">
+        <v>231</v>
+      </c>
+      <c r="C21" s="136">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C22" s="138">
+        <v>222</v>
+      </c>
+      <c r="C22" s="136">
         <v>-6</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C23" s="138">
+        <v>221</v>
+      </c>
+      <c r="C23" s="136">
         <v>-5</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" s="138">
+        <v>232</v>
+      </c>
+      <c r="C24" s="136">
         <v>470</v>
       </c>
     </row>
     <row r="25" spans="2:3">
       <c r="B25" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="C25" s="138">
+        <v>222</v>
+      </c>
+      <c r="C25" s="136">
         <v>-49</v>
       </c>
     </row>
     <row r="26" spans="2:3">
       <c r="B26" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C26" s="138">
+        <v>221</v>
+      </c>
+      <c r="C26" s="136">
         <v>-82</v>
       </c>
     </row>
@@ -3959,7 +4132,7 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9" style="27"/>
-    <col min="2" max="2" width="3.75" style="128" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="126" customWidth="1"/>
     <col min="3" max="3" width="7.375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.625" style="27" customWidth="1"/>
     <col min="6" max="6" width="1.875" style="27" bestFit="1" customWidth="1"/>
@@ -3970,370 +4143,381 @@
   <sheetData>
     <row r="2" spans="2:9" ht="16.5" thickBot="1"/>
     <row r="3" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B3" s="194" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
+      <c r="B3" s="171" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="172"/>
+      <c r="D3" s="173"/>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="130" t="s">
+      <c r="B4" s="129" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="128" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="132" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="132" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="132" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="132" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="135"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="132" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D11" s="132" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="134" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="134" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="134" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" s="134" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D12" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="131" t="s">
         <v>133</v>
-      </c>
-      <c r="D9" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" s="134" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" s="137"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="134" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="133" t="s">
-        <v>140</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="134" t="s">
-        <v>126</v>
+      <c r="D13" s="132" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="27" customHeight="1" thickBot="1">
-      <c r="B14" s="135" t="s">
+      <c r="B14" s="133" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="134" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18.75" customHeight="1">
+      <c r="B15" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="174" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="175"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="167" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="168"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="167" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="168"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B18" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="168"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B19" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="167" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="168"/>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B20" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="167" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="168"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B21" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="167" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="168"/>
+    </row>
+    <row r="22" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B22" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="167" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="168"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="167" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="168"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="167" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="168"/>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B25" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="167" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="168"/>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B26" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="167" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="168"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="167" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="168"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="167" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="168"/>
+    </row>
+    <row r="29" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B29" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="167" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="168"/>
+    </row>
+    <row r="30" spans="2:4" ht="33" customHeight="1">
+      <c r="B30" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="167" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="168"/>
+    </row>
+    <row r="31" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B31" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="167" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="168"/>
+    </row>
+    <row r="32" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B32" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="167" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="168"/>
+    </row>
+    <row r="33" spans="2:4" ht="34.5" customHeight="1">
+      <c r="B33" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="167" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="168"/>
+    </row>
+    <row r="34" spans="2:4" ht="32.25" customHeight="1">
+      <c r="B34" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="167" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="168"/>
+    </row>
+    <row r="35" spans="2:4" ht="31.5" customHeight="1">
+      <c r="B35" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="167" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="168"/>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B36" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="167" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="168"/>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B37" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="167" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="168"/>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B38" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" s="167" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="168"/>
+    </row>
+    <row r="39" spans="2:4" ht="37.5" customHeight="1">
+      <c r="B39" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="167" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="168"/>
+    </row>
+    <row r="40" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B40" s="133" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" s="169" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="129" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="136" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="18.75" customHeight="1">
-      <c r="B15" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="190" t="s">
-        <v>138</v>
-      </c>
-      <c r="D15" s="191"/>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="188" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="189"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="188" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="189"/>
-    </row>
-    <row r="18" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B18" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="188" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="189"/>
-    </row>
-    <row r="19" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B19" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="188" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="189"/>
-    </row>
-    <row r="20" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B20" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="188" t="s">
-        <v>152</v>
-      </c>
-      <c r="D20" s="189"/>
-    </row>
-    <row r="21" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B21" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="188" t="s">
-        <v>153</v>
-      </c>
-      <c r="D21" s="189"/>
-    </row>
-    <row r="22" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B22" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="188" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="189"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="188" t="s">
-        <v>154</v>
-      </c>
-      <c r="D23" s="189"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="188" t="s">
-        <v>155</v>
-      </c>
-      <c r="D24" s="189"/>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B25" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="188" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="189"/>
-    </row>
-    <row r="26" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B26" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="188" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="189"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="188" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="189"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="188" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="189"/>
-    </row>
-    <row r="29" spans="2:4" ht="33.75" customHeight="1">
-      <c r="B29" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="188" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="189"/>
-    </row>
-    <row r="30" spans="2:4" ht="33" customHeight="1">
-      <c r="B30" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="188" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="189"/>
-    </row>
-    <row r="31" spans="2:4" ht="33.75" customHeight="1">
-      <c r="B31" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="188" t="s">
-        <v>160</v>
-      </c>
-      <c r="D31" s="189"/>
-    </row>
-    <row r="32" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B32" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="188" t="s">
-        <v>161</v>
-      </c>
-      <c r="D32" s="189"/>
-    </row>
-    <row r="33" spans="2:4" ht="34.5" customHeight="1">
-      <c r="B33" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C33" s="188" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="189"/>
-    </row>
-    <row r="34" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B34" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="188" t="s">
-        <v>163</v>
-      </c>
-      <c r="D34" s="189"/>
-    </row>
-    <row r="35" spans="2:4" ht="31.5" customHeight="1">
-      <c r="B35" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C35" s="188" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35" s="189"/>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B36" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="188" t="s">
-        <v>148</v>
-      </c>
-      <c r="D36" s="189"/>
-    </row>
-    <row r="37" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B37" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C37" s="188" t="s">
-        <v>149</v>
-      </c>
-      <c r="D37" s="189"/>
-    </row>
-    <row r="38" spans="2:4" ht="15.75" customHeight="1">
-      <c r="B38" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C38" s="188" t="s">
-        <v>150</v>
-      </c>
-      <c r="D38" s="189"/>
-    </row>
-    <row r="39" spans="2:4" ht="37.5" customHeight="1">
-      <c r="B39" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="188" t="s">
-        <v>165</v>
-      </c>
-      <c r="D39" s="189"/>
-    </row>
-    <row r="40" spans="2:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B40" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="192" t="s">
-        <v>147</v>
-      </c>
-      <c r="D40" s="193"/>
+      <c r="D40" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
@@ -4350,17 +4534,6 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
@@ -4387,257 +4560,252 @@
   <sheetData>
     <row r="2" spans="2:4" ht="16.5" thickBot="1"/>
     <row r="3" spans="2:4" ht="16.5" thickBot="1">
-      <c r="B3" s="194" t="s">
+      <c r="B3" s="171" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="172"/>
+      <c r="D3" s="173"/>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="129" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="128" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="132" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="132" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="132" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="132" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="132" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="130" t="s">
+      <c r="D12" s="132" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="132" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="16.5" thickBot="1">
+      <c r="B14" s="133" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="134" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="129" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="174" t="s">
+        <v>177</v>
+      </c>
+      <c r="D15" s="175"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="167" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="168"/>
+    </row>
+    <row r="17" spans="2:4" ht="34.5" customHeight="1">
+      <c r="B17" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="167" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="168"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="168"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="167" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="168"/>
+    </row>
+    <row r="20" spans="2:4" ht="39" customHeight="1">
+      <c r="B20" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="167" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="168"/>
+    </row>
+    <row r="21" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B21" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="167" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="168"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="167" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="132" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="134" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="134" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="134" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="134" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D10" s="134" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" s="134" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D12" s="134" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D13" s="134" t="s">
+      <c r="D22" s="168"/>
+    </row>
+    <row r="23" spans="2:4" ht="37.5" customHeight="1">
+      <c r="B23" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="167" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" s="168"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="167" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="16.5" thickBot="1">
-      <c r="B14" s="135" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="129" t="s">
-        <v>175</v>
-      </c>
-      <c r="D14" s="136" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="131" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="190" t="s">
+      <c r="D24" s="168"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="167" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25" s="168"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="167" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="168"/>
+    </row>
+    <row r="27" spans="2:4" ht="16.5" thickBot="1">
+      <c r="B27" s="133" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="169" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="191"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C16" s="188" t="s">
-        <v>185</v>
-      </c>
-      <c r="D16" s="189"/>
-    </row>
-    <row r="17" spans="2:4" ht="34.5" customHeight="1">
-      <c r="B17" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="188" t="s">
-        <v>220</v>
-      </c>
-      <c r="D17" s="189"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="188" t="s">
-        <v>186</v>
-      </c>
-      <c r="D18" s="189"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="188" t="s">
-        <v>187</v>
-      </c>
-      <c r="D19" s="189"/>
-    </row>
-    <row r="20" spans="2:4" ht="39" customHeight="1">
-      <c r="B20" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="188" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="189"/>
-    </row>
-    <row r="21" spans="2:4" ht="33.75" customHeight="1">
-      <c r="B21" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="188" t="s">
-        <v>219</v>
-      </c>
-      <c r="D21" s="189"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="188" t="s">
-        <v>189</v>
-      </c>
-      <c r="D22" s="189"/>
-    </row>
-    <row r="23" spans="2:4" ht="37.5" customHeight="1">
-      <c r="B23" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="188" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="189"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="188" t="s">
-        <v>190</v>
-      </c>
-      <c r="D24" s="189"/>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="188" t="s">
-        <v>216</v>
-      </c>
-      <c r="D25" s="189"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="188" t="s">
-        <v>217</v>
-      </c>
-      <c r="D26" s="189"/>
-    </row>
-    <row r="27" spans="2:4" ht="16.5" thickBot="1">
-      <c r="B27" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="192" t="s">
-        <v>191</v>
-      </c>
-      <c r="D27" s="193"/>
+      <c r="D27" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
@@ -4647,6 +4815,11 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4673,298 +4846,293 @@
   <sheetData>
     <row r="2" spans="2:6" ht="16.5" thickBot="1"/>
     <row r="3" spans="2:6" ht="16.5" thickBot="1">
-      <c r="B3" s="194" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
+      <c r="B3" s="171" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="172"/>
+      <c r="D3" s="173"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="130" t="s">
+      <c r="B4" s="129" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="128" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="132" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="132" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D9" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D4" s="132" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D10" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="D5" s="134" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="D11" s="132" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="134" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D12" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="132" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="132" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D15" s="132" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="16.5" thickBot="1">
+      <c r="B16" s="133" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="127" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="134" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="129" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="174" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="175"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="167" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="168"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="167" t="s">
+        <v>202</v>
+      </c>
+      <c r="D19" s="168"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="167" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="168"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="167" t="s">
+        <v>204</v>
+      </c>
+      <c r="D21" s="168"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="167" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="168"/>
+    </row>
+    <row r="23" spans="2:4" ht="36" customHeight="1">
+      <c r="B23" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="167" t="s">
         <v>206</v>
       </c>
-      <c r="D7" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D8" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D10" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D11" s="134" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D12" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D13" s="134" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D14" s="134" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="133" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D15" s="134" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="16.5" thickBot="1">
-      <c r="B16" s="135" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" s="129" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="136" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="131" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="190" t="s">
+      <c r="D23" s="168"/>
+    </row>
+    <row r="24" spans="2:4" ht="32.25" customHeight="1">
+      <c r="B24" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="167" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="191"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="188" t="s">
+      <c r="D24" s="168"/>
+    </row>
+    <row r="25" spans="2:4" ht="33.75" customHeight="1">
+      <c r="B25" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" s="167" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="168"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="167" t="s">
         <v>208</v>
       </c>
-      <c r="D18" s="189"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C19" s="188" t="s">
-        <v>209</v>
-      </c>
-      <c r="D19" s="189"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="188" t="s">
-        <v>210</v>
-      </c>
-      <c r="D20" s="189"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C21" s="188" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="189"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="188" t="s">
-        <v>212</v>
-      </c>
-      <c r="D22" s="189"/>
-    </row>
-    <row r="23" spans="2:4" ht="36" customHeight="1">
-      <c r="B23" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="188" t="s">
-        <v>213</v>
-      </c>
-      <c r="D23" s="189"/>
-    </row>
-    <row r="24" spans="2:4" ht="32.25" customHeight="1">
-      <c r="B24" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="188" t="s">
+      <c r="D26" s="168"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="167" t="s">
+        <v>219</v>
+      </c>
+      <c r="D27" s="168"/>
+    </row>
+    <row r="28" spans="2:4" ht="29.25" customHeight="1">
+      <c r="B28" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="167" t="s">
         <v>214</v>
       </c>
-      <c r="D24" s="189"/>
-    </row>
-    <row r="25" spans="2:4" ht="33.75" customHeight="1">
-      <c r="B25" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C25" s="188" t="s">
-        <v>225</v>
-      </c>
-      <c r="D25" s="189"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="188" t="s">
+      <c r="D28" s="168"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="167" t="s">
         <v>215</v>
       </c>
-      <c r="D26" s="189"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="188" t="s">
-        <v>226</v>
-      </c>
-      <c r="D27" s="189"/>
-    </row>
-    <row r="28" spans="2:4" ht="29.25" customHeight="1">
-      <c r="B28" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="188" t="s">
-        <v>221</v>
-      </c>
-      <c r="D28" s="189"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="188" t="s">
-        <v>222</v>
-      </c>
-      <c r="D29" s="189"/>
+      <c r="D29" s="168"/>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="133" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="188" t="s">
-        <v>223</v>
-      </c>
-      <c r="D30" s="189"/>
+      <c r="B30" s="131" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="167" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" s="168"/>
     </row>
     <row r="31" spans="2:4" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B31" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="192" t="s">
-        <v>224</v>
-      </c>
-      <c r="D31" s="193"/>
+      <c r="B31" s="133" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="169" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="C17:D17"/>
@@ -4976,6 +5144,11 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4983,607 +5156,671 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5F16840-50DC-4E6F-A125-B5573596E681}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDB327B-5EAE-4B83-A410-DD0AD4C5EA34}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="143" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="43" workbookViewId="0">
+      <selection sqref="A1:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57" style="4" customWidth="1"/>
+    <col min="4" max="4" width="65.875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.625" style="22" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25">
-      <c r="A1" s="160" t="s">
+      <c r="A1" s="228" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="230"/>
     </row>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="231" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-    </row>
-    <row r="3" spans="1:12" ht="21.75" thickBot="1">
-      <c r="A3" s="162" t="s">
+      <c r="B2" s="232"/>
+      <c r="C2" s="232"/>
+      <c r="D2" s="233"/>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A3" s="234"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="235"/>
+    </row>
+    <row r="4" spans="1:12" ht="21.75" thickBot="1">
+      <c r="A4" s="236" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
-      <c r="I3" s="154"/>
-      <c r="J3" s="154"/>
-      <c r="K3" s="154"/>
-      <c r="L3" s="154"/>
-    </row>
-    <row r="4" spans="1:12" ht="23.25">
-      <c r="A4" s="200"/>
-      <c r="B4" s="202" t="s">
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="237"/>
+      <c r="F4" s="145" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="147"/>
+    </row>
+    <row r="5" spans="1:12" ht="23.25">
+      <c r="A5" s="238"/>
+      <c r="B5" s="239" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="202"/>
-      <c r="D4" s="203"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A5" s="201"/>
-      <c r="B5" s="166" t="s">
+      <c r="C5" s="239"/>
+      <c r="D5" s="240"/>
+      <c r="F5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="149" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="149"/>
+      <c r="I5" s="149"/>
+      <c r="J5" s="149"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="149"/>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A6" s="238"/>
+      <c r="B6" s="241" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="166"/>
-      <c r="D5" s="204"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-    </row>
-    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A6" s="201"/>
-      <c r="B6" s="166"/>
-      <c r="C6" s="166"/>
-      <c r="D6" s="204"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
+      <c r="C6" s="241"/>
+      <c r="D6" s="242"/>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="150" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="150"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="150"/>
+      <c r="K6" s="150"/>
+      <c r="L6" s="150"/>
     </row>
     <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="238"/>
+      <c r="B7" s="241"/>
+      <c r="C7" s="241"/>
+      <c r="D7" s="242"/>
+      <c r="F7" s="154" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="148" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="148"/>
+      <c r="I7" s="148"/>
+      <c r="J7" s="148"/>
+      <c r="K7" s="148"/>
+      <c r="L7" s="148"/>
+    </row>
+    <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1">
+      <c r="A8" s="188" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="197" t="s">
+      <c r="B8" s="176" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="198"/>
-      <c r="D7" s="199"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="189"/>
+      <c r="D8" s="190"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="148"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="148"/>
+      <c r="J8" s="148"/>
+      <c r="K8" s="148"/>
+      <c r="L8" s="148"/>
+    </row>
+    <row r="9" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1">
+      <c r="A9" s="191"/>
+      <c r="B9" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="31" t="s">
+      <c r="C9" s="193"/>
+      <c r="D9" s="194" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" ht="24" thickBot="1">
-      <c r="A9" s="155"/>
-      <c r="B9" s="147" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" ht="24" thickBot="1">
+      <c r="A10" s="243"/>
+      <c r="B10" s="195" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="148" t="s">
+      <c r="C10" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="149"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="47.25" thickBot="1">
-      <c r="A10" s="158" t="s">
+      <c r="D10" s="197"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="24" thickBot="1">
+      <c r="A11" s="198" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="176"/>
-      <c r="C10" s="176"/>
-      <c r="D10" s="177"/>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="23.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="199"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="200"/>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25">
+      <c r="A12" s="201"/>
+      <c r="B12" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="179"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="1:12" ht="23.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="203"/>
+      <c r="D12" s="204" t="s">
+        <v>235</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:12" ht="23.25">
+      <c r="A13" s="205"/>
+      <c r="B13" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="207" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="33">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="23.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="28" t="s">
+      <c r="D13" s="208" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="23.25">
+      <c r="A14" s="205"/>
+      <c r="B14" s="209" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C14" s="210" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="150"/>
-    </row>
-    <row r="14" spans="1:12" ht="23.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="9" t="s">
+      <c r="D14" s="211"/>
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" spans="1:12" ht="23.25">
+      <c r="A15" s="205"/>
+      <c r="B15" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="33"/>
-    </row>
-    <row r="15" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="167" t="s">
+      <c r="D15" s="208"/>
+    </row>
+    <row r="16" spans="1:12" ht="23.25" customHeight="1">
+      <c r="A16" s="212"/>
+      <c r="B16" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="168"/>
-      <c r="D15" s="169"/>
-    </row>
-    <row r="16" spans="1:12" ht="23.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="9" t="s">
+      <c r="C16" s="214"/>
+      <c r="D16" s="204" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="23.25">
+      <c r="A17" s="205"/>
+      <c r="B17" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="33">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="23.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="9" t="s">
+      <c r="D17" s="208" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="23.25">
+      <c r="A18" s="205"/>
+      <c r="B18" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="207" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="33">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="23.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="9" t="s">
+      <c r="D18" s="208">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="23.25">
+      <c r="A19" s="205"/>
+      <c r="B19" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="207" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="33"/>
-    </row>
-    <row r="19" spans="1:6" ht="23.25" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="167" t="s">
+      <c r="D19" s="208"/>
+    </row>
+    <row r="20" spans="1:6" ht="23.25" customHeight="1">
+      <c r="A20" s="212"/>
+      <c r="B20" s="213" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="168"/>
-      <c r="D19" s="169"/>
-    </row>
-    <row r="20" spans="1:6" ht="23.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="214"/>
+      <c r="D20" s="204" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="23.25">
+      <c r="A21" s="205"/>
+      <c r="B21" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="207" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="33">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="23.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="9" t="s">
+      <c r="D21" s="208">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="23.25">
+      <c r="A22" s="205"/>
+      <c r="B22" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="207" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="33"/>
-      <c r="E21"/>
-    </row>
-    <row r="22" spans="1:6" ht="24" thickBot="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18" t="s">
+      <c r="D22" s="208" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" thickBot="1">
+      <c r="A23" s="215"/>
+      <c r="B23" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C23" s="217" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="34"/>
-    </row>
-    <row r="23" spans="1:6" ht="24" thickBot="1">
-      <c r="A23" s="159" t="s">
+      <c r="D23" s="218"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" thickBot="1">
+      <c r="A24" s="198" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="176"/>
-      <c r="C23" s="176"/>
-      <c r="D23" s="177"/>
-      <c r="E23" s="1"/>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" ht="23.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="178" t="s">
+      <c r="B24" s="199"/>
+      <c r="C24" s="199"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="125" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" ht="23.25">
+      <c r="A25" s="201"/>
+      <c r="B25" s="219" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="179"/>
-      <c r="D24" s="180"/>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" ht="23.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="220"/>
+      <c r="D25" s="204" t="s">
+        <v>235</v>
+      </c>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" ht="93.75">
+      <c r="A26" s="205"/>
+      <c r="B26" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="207" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="156" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="25"/>
-    </row>
-    <row r="26" spans="1:6" ht="23.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="9" t="s">
+      <c r="D26" s="244" t="s">
+        <v>245</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="23.25">
+      <c r="A27" s="205"/>
+      <c r="B27" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="207" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="23.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="9" t="s">
+      <c r="D27" s="208" t="s">
+        <v>244</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="1">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="37.5">
+      <c r="A28" s="205"/>
+      <c r="B28" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C28" s="207" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="E27" s="44"/>
-    </row>
-    <row r="28" spans="1:6" ht="23.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="9" t="s">
+      <c r="D28" s="208" t="s">
+        <v>247</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="1">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="23.25">
+      <c r="A29" s="205"/>
+      <c r="B29" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="207" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" ht="23.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="9" t="s">
+      <c r="D29" s="208" t="s">
+        <v>241</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="23.25">
+      <c r="A30" s="205"/>
+      <c r="B30" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="207" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="157" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" ht="24" thickBot="1">
-      <c r="A30" s="17"/>
-      <c r="B30" s="9" t="s">
+      <c r="D30" s="245" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="1">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="38.25" thickBot="1">
+      <c r="A31" s="215"/>
+      <c r="B31" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C31" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="25"/>
-    </row>
-    <row r="31" spans="1:6" ht="24" thickBot="1">
-      <c r="A31" s="159" t="s">
+      <c r="D31" s="208" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="24" thickBot="1">
+      <c r="A32" s="198" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="171" t="s">
+      <c r="B32" s="221" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="171"/>
-      <c r="D31" s="181"/>
-    </row>
-    <row r="32" spans="1:6" s="22" customFormat="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="178" t="s">
+      <c r="C32" s="221"/>
+      <c r="D32" s="222"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="223"/>
+      <c r="B33" s="202" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="179"/>
-      <c r="D32" s="180"/>
-    </row>
-    <row r="33" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="9" t="s">
+      <c r="C33" s="203"/>
+      <c r="D33" s="204" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="23.25">
+      <c r="A34" s="205"/>
+      <c r="B34" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="207" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="33"/>
-    </row>
-    <row r="34" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="9" t="s">
+      <c r="D34" s="208"/>
+    </row>
+    <row r="35" spans="1:4" ht="23.25">
+      <c r="A35" s="205"/>
+      <c r="B35" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="207" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="33">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="9" t="s">
+      <c r="D35" s="208">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="23.25">
+      <c r="A36" s="205"/>
+      <c r="B36" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="207" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="33"/>
-    </row>
-    <row r="36" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="9" t="s">
+      <c r="D36" s="208"/>
+    </row>
+    <row r="37" spans="1:4" ht="23.25">
+      <c r="A37" s="205"/>
+      <c r="B37" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="207" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="33"/>
-    </row>
-    <row r="37" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="9" t="s">
+      <c r="D37" s="208"/>
+    </row>
+    <row r="38" spans="1:4" ht="23.25">
+      <c r="A38" s="205"/>
+      <c r="B38" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="207" t="s">
         <v>35</v>
       </c>
-      <c r="D37" s="33"/>
-    </row>
-    <row r="38" spans="1:4" s="22" customFormat="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="167" t="s">
+      <c r="D38" s="208"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="205"/>
+      <c r="B39" s="213" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
-    </row>
-    <row r="39" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="9" t="s">
+      <c r="C39" s="214"/>
+      <c r="D39" s="204" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.25">
+      <c r="A40" s="205"/>
+      <c r="B40" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="207" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="33">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="9" t="s">
+      <c r="D40" s="208" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="23.25">
+      <c r="A41" s="205"/>
+      <c r="B41" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C41" s="207" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="33"/>
-    </row>
-    <row r="41" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="9" t="s">
+      <c r="D41" s="208"/>
+    </row>
+    <row r="42" spans="1:4" ht="23.25">
+      <c r="A42" s="205"/>
+      <c r="B42" s="206" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="207" t="s">
         <v>39</v>
       </c>
-      <c r="D41" s="33"/>
-    </row>
-    <row r="42" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="9" t="s">
+      <c r="D42" s="208">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="23.25">
+      <c r="A43" s="205"/>
+      <c r="B43" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="207" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="33"/>
-    </row>
-    <row r="43" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="9" t="s">
+      <c r="D43" s="208"/>
+    </row>
+    <row r="44" spans="1:4" ht="23.25">
+      <c r="A44" s="205"/>
+      <c r="B44" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C44" s="207" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="33"/>
-    </row>
-    <row r="44" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="9" t="s">
+      <c r="D44" s="208"/>
+    </row>
+    <row r="45" spans="1:4" ht="23.25">
+      <c r="A45" s="205"/>
+      <c r="B45" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C45" s="207" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="33"/>
-    </row>
-    <row r="45" spans="1:4" s="22" customFormat="1" ht="24" thickBot="1">
-      <c r="A45" s="14"/>
-      <c r="B45" s="9" t="s">
+      <c r="D45" s="208"/>
+    </row>
+    <row r="46" spans="1:4" ht="23.25">
+      <c r="A46" s="205"/>
+      <c r="B46" s="206" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="207" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="208" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="205"/>
+      <c r="B47" s="213" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="214"/>
+      <c r="D47" s="204" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="23.25">
+      <c r="A48" s="205"/>
+      <c r="B48" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="33"/>
-    </row>
-    <row r="46" spans="1:4" s="22" customFormat="1">
-      <c r="A46" s="14"/>
-      <c r="B46" s="167" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="168"/>
-      <c r="D46" s="169"/>
-    </row>
-    <row r="47" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="9" t="s">
+      <c r="C48" s="207" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="208"/>
+    </row>
+    <row r="49" spans="1:4" ht="23.25">
+      <c r="A49" s="205"/>
+      <c r="B49" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="33"/>
-    </row>
-    <row r="48" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="9" t="s">
+      <c r="C49" s="207" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="208"/>
+    </row>
+    <row r="50" spans="1:4" ht="23.25">
+      <c r="A50" s="205"/>
+      <c r="B50" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="33"/>
-    </row>
-    <row r="49" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="9" t="s">
+      <c r="C50" s="207" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="208"/>
+    </row>
+    <row r="51" spans="1:4" ht="23.25">
+      <c r="A51" s="205"/>
+      <c r="B51" s="206" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="33"/>
-    </row>
-    <row r="50" spans="1:4" s="22" customFormat="1" ht="23.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="207" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="33"/>
-    </row>
-    <row r="51" spans="1:4" s="22" customFormat="1" ht="24" thickBot="1">
-      <c r="A51" s="15"/>
-      <c r="B51" s="151" t="s">
+      <c r="D51" s="208"/>
+    </row>
+    <row r="52" spans="1:4" ht="24" thickBot="1">
+      <c r="A52" s="224"/>
+      <c r="B52" s="225" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="126" t="s">
+      <c r="C52" s="226" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="127" t="s">
-        <v>118</v>
+      <c r="D52" s="227" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:L8"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D6"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="B6:D7"/>
+    <mergeCell ref="G6:L6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{48A79B56-9EDB-4A9B-992E-539D7A011C79}"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{518891C4-3E26-403A-849B-F34317852392}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="30" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>